<commit_message>
Add multi-command, toggle, and cmdhold support for checklist commands column
Commands column now supports semicolon-separated commands, toggle: prefix
(checks dataref before firing), and cmdhold: prefix (begin/end for rotary
switches). Also fixes ScriptExecutor not defined error in label-guess path.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/CopilotAI_Checklists.xlsx
+++ b/CopilotAI_Checklists.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnl\Documents\projects\CopilotAI\claude_shell_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D949772-7191-440E-A861-9EBB8D48B05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10000001_{29E35F33-D669-4A3D-A249-8BDE24226DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57840" yWindow="-98" windowWidth="28995" windowHeight="16395" xr2:uid="{B7C423D5-FDD5-4D99-96F7-653924CCE03F}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="ZIBO737" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="230">
   <si>
     <t>checklist</t>
   </si>
@@ -73,9 +74,6 @@
     <t>ON and GUARDED</t>
   </si>
   <si>
-    <t>{(sim/cockpit2/electrical/battery_on[0]:1)&amp;&amp;(laminar/B738/button_switch/cover_position[2]:0)&amp;&amp;(sim/operation/failures/rel_batter0:0)}</t>
-  </si>
-  <si>
     <t>APU START</t>
   </si>
   <si>
@@ -508,9 +506,6 @@
     <t>Cockpit Deck Door</t>
   </si>
   <si>
-    <t>laminar/B738/fms/chock_status:1.0</t>
-  </si>
-  <si>
     <t>BLOCK</t>
   </si>
   <si>
@@ -628,7 +623,94 @@
     <t>APU</t>
   </si>
   <si>
-    <t>(laminar/B738/toggle_switch/capt_probes_pos:1.0)&amp;&amp;(sim/operation/failures/rel_ice_pitot_heat1:0)&amp;&amp;(laminar/B738/toggle_switch/fo_probes_pos:1.0)&amp;&amp;(sim/operation/failures/rel_ice_pitot_heat1:0)</t>
+    <t>CONTINUOUS</t>
+  </si>
+  <si>
+    <t>FLAPS</t>
+  </si>
+  <si>
+    <t>TAXI LIGHTS</t>
+  </si>
+  <si>
+    <t>(laminar/B738/toggle_switch/taxi_light_brightness_pos:&gt;0.0)&amp;&amp;(sim/operation/failures/rel_lites_taxi:0)</t>
+  </si>
+  <si>
+    <t>YAW DAMPER</t>
+  </si>
+  <si>
+    <t>ENGINE START</t>
+  </si>
+  <si>
+    <t>cmdhold:0.5:laminar/B738/rotary/eng1_start_cont; cmdhold:laminar/B738/rotary/eng2_start_cont;</t>
+  </si>
+  <si>
+    <t>toggle:laminar/B738/toggle_switch/yaw_dumper=laminar/B738/toggle_switch/yaw_dumper_pos:1;</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/push_button/flaps_5</t>
+  </si>
+  <si>
+    <t>TAXI</t>
+  </si>
+  <si>
+    <t>TAKEOFF</t>
+  </si>
+  <si>
+    <t>laminar/B738/toggle_switch/taxi_light_brightness_pos:0.0</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/taxi_light_brigh_toggle</t>
+  </si>
+  <si>
+    <t>LANDING LIGHT</t>
+  </si>
+  <si>
+    <t>POSITION LIGHTS</t>
+  </si>
+  <si>
+    <t>STROBE</t>
+  </si>
+  <si>
+    <t>TARA</t>
+  </si>
+  <si>
+    <t>laminar/B738/knob/transponder_pos:5</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/position_light_strobe</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/knob/transponder_tara</t>
+  </si>
+  <si>
+    <t>set:laminar/B738/fms/chock_status=1;</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/push_button/park_brake_on_off</t>
+  </si>
+  <si>
+    <t>laminar/B738/annunciator/parking_brake:&gt;0.01</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/gpu_toggle</t>
+  </si>
+  <si>
+    <t>laminar/B738/gpu_available:1.0</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/button_switch_cover02</t>
+  </si>
+  <si>
+    <t>laminar/B738/button_switch/cover_position[2]:0</t>
+  </si>
+  <si>
+    <t>set:laminar/B738/toggle_switch/capt_probes_pos=1; set:laminar/B738/toggle_switch/fo_probes_pos=1;</t>
+  </si>
+  <si>
+    <t>(laminar/B738/toggle_switch/capt_probes_pos:1.0)&amp;&amp;(laminar/B738/toggle_switch/fo_probes_pos:1.0)</t>
+  </si>
+  <si>
+    <t>set:laminar/B738/switch/land_lights_left_pos=1; set:laminar/B738/switch/land_lights_right_pos=1;</t>
   </si>
 </sst>
 </file>
@@ -1228,22 +1310,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}" name="ZIBO737" displayName="ZIBO737" ref="A1:M75" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:M75" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}" name="ZIBO737" displayName="ZIBO737" ref="A1:M87" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:M87" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{D7EB0E30-B8BB-40E3-B6DB-C78633A8AE10}" name="checklist" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{3F7C8B58-5F6F-4EDC-93DE-0EFE3A81396D}" name="enabled" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{01D1E4D6-1DB5-47B3-AAB3-A1B68150B44F}" name="group" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{72FFAAE9-5D8C-40EB-AE40-8F469B0E7D59}" name="order" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{920337F0-56EA-4F1F-986B-102213412169}" name="group2" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{36676C6C-49EA-4FF9-8E63-6BEF44843C00}" name="type" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{460E5C61-EEC5-4F96-9F6B-BAE749518F16}" name="label" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{197D6612-0EC9-4731-A70B-559CA562709F}" name="status_text" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{077D9AF1-4A41-4A35-8CA8-A7F43BA57B29}" name="speak" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{BF0DE601-6A90-4914-943B-FB3758618C69}" name="speak_on" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{58980946-BD94-4B4D-B114-12165AE8D78E}" name="conditions" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{6283B833-A799-4A62-B487-95ED808B28CD}" name="commands" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{E1F6A41E-D7AD-4672-B6E5-6DABB0756EF2}" name="notes" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{3F7C8B58-5F6F-4EDC-93DE-0EFE3A81396D}" name="enabled" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{01D1E4D6-1DB5-47B3-AAB3-A1B68150B44F}" name="group" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{72FFAAE9-5D8C-40EB-AE40-8F469B0E7D59}" name="order" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{920337F0-56EA-4F1F-986B-102213412169}" name="group2" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{36676C6C-49EA-4FF9-8E63-6BEF44843C00}" name="type" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{460E5C61-EEC5-4F96-9F6B-BAE749518F16}" name="label" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{197D6612-0EC9-4731-A70B-559CA562709F}" name="status_text" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{077D9AF1-4A41-4A35-8CA8-A7F43BA57B29}" name="speak" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{BF0DE601-6A90-4914-943B-FB3758618C69}" name="speak_on" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{58980946-BD94-4B4D-B114-12165AE8D78E}" name="conditions" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{6283B833-A799-4A62-B487-95ED808B28CD}" name="commands" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{E1F6A41E-D7AD-4672-B6E5-6DABB0756EF2}" name="notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1566,11 +1648,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BB3736-AF94-49F8-BA64-38BE7B846CBA}">
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K70" sqref="K70"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L77" sqref="L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1605,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1634,7 +1716,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1646,27 +1728,27 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -1678,27 +1760,27 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -1710,27 +1792,27 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1742,27 +1824,27 @@
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -1774,27 +1856,27 @@
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1806,27 +1888,27 @@
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -1838,27 +1920,27 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="L8" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1870,27 +1952,27 @@
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -1902,28 +1984,27 @@
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L10" s="1"/>
+      <c r="L10" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -1935,25 +2016,30 @@
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>23</v>
+        <v>167</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="K11" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -1965,25 +2051,27 @@
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>169</v>
+        <v>22</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="L12" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -1995,25 +2083,27 @@
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>168</v>
+        <v>24</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="L13" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -2025,85 +2115,88 @@
         <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>25</v>
+        <v>168</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="L14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>14</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="L15" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>143</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -2114,29 +2207,31 @@
         <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>164</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>15</v>
+        <v>139</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L17" s="1"/>
+        <v>222</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -2147,7 +2242,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>13</v>
@@ -2156,19 +2251,19 @@
         <v>14</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
@@ -2182,7 +2277,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>13</v>
@@ -2191,15 +2286,15 @@
         <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -2215,24 +2310,24 @@
         <v>2</v>
       </c>
       <c r="D20" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="L20" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M20" s="1"/>
     </row>
@@ -2247,19 +2342,19 @@
         <v>2</v>
       </c>
       <c r="D21" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2278,7 +2373,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>13</v>
@@ -2287,15 +2382,15 @@
         <v>14</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -2311,24 +2406,24 @@
         <v>2</v>
       </c>
       <c r="D23" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -2344,24 +2439,24 @@
         <v>2</v>
       </c>
       <c r="D24" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -2377,24 +2472,24 @@
         <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2410,24 +2505,24 @@
         <v>2</v>
       </c>
       <c r="D26" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2443,24 +2538,24 @@
         <v>2</v>
       </c>
       <c r="D27" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2476,24 +2571,24 @@
         <v>2</v>
       </c>
       <c r="D28" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="H28" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2509,24 +2604,24 @@
         <v>2</v>
       </c>
       <c r="D29" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="H29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -2542,24 +2637,24 @@
         <v>2</v>
       </c>
       <c r="D30" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -2575,24 +2670,24 @@
         <v>2</v>
       </c>
       <c r="D31" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -2608,24 +2703,24 @@
         <v>2</v>
       </c>
       <c r="D32" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -2641,24 +2736,24 @@
         <v>2</v>
       </c>
       <c r="D33" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -2674,24 +2769,24 @@
         <v>2</v>
       </c>
       <c r="D34" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="H34" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -2707,24 +2802,24 @@
         <v>2</v>
       </c>
       <c r="D35" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2740,24 +2835,24 @@
         <v>2</v>
       </c>
       <c r="D36" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -2773,24 +2868,24 @@
         <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -2806,24 +2901,24 @@
         <v>2</v>
       </c>
       <c r="D38" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2839,24 +2934,24 @@
         <v>2</v>
       </c>
       <c r="D39" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -2872,24 +2967,24 @@
         <v>2</v>
       </c>
       <c r="D40" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -2905,24 +3000,24 @@
         <v>2</v>
       </c>
       <c r="D41" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2938,24 +3033,24 @@
         <v>2</v>
       </c>
       <c r="D42" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -2974,21 +3069,21 @@
         <v>28</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -3007,21 +3102,21 @@
         <v>29</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="H44" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -3040,21 +3135,21 @@
         <v>30</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="H45" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -3073,21 +3168,21 @@
         <v>31</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="H46" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -3106,21 +3201,21 @@
         <v>32</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -3139,21 +3234,21 @@
         <v>33</v>
       </c>
       <c r="E48" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -3173,10 +3268,10 @@
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -3186,7 +3281,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -3198,28 +3293,28 @@
         <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B51" s="1">
         <v>1</v>
@@ -3231,28 +3326,28 @@
         <v>2</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B52" s="1">
         <v>1</v>
@@ -3265,10 +3360,10 @@
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -3278,7 +3373,7 @@
     </row>
     <row r="53" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B53" s="1">
         <v>1</v>
@@ -3290,28 +3385,28 @@
         <v>1</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
     </row>
     <row r="54" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B54" s="1">
         <v>1</v>
@@ -3323,28 +3418,28 @@
         <v>2</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G54" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B55" s="1">
         <v>1</v>
@@ -3356,28 +3451,28 @@
         <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G55" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B56" s="1">
         <v>1</v>
@@ -3389,28 +3484,28 @@
         <v>4</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G56" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
@@ -3422,28 +3517,28 @@
         <v>5</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G57" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B58" s="1">
         <v>1</v>
@@ -3456,10 +3551,10 @@
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -3469,7 +3564,7 @@
     </row>
     <row r="59" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B59" s="1">
         <v>1</v>
@@ -3481,28 +3576,28 @@
         <v>1</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
     </row>
     <row r="60" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B60" s="1">
         <v>1</v>
@@ -3514,28 +3609,28 @@
         <v>2</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B61" s="1">
         <v>1</v>
@@ -3547,28 +3642,28 @@
         <v>3</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G61" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B62" s="1">
         <v>1</v>
@@ -3580,28 +3675,28 @@
         <v>4</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B63" s="1">
         <v>1</v>
@@ -3613,28 +3708,28 @@
         <v>5</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
     </row>
     <row r="64" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
@@ -3646,28 +3741,28 @@
         <v>6</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
     <row r="65" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B65" s="1">
         <v>1</v>
@@ -3685,22 +3780,22 @@
         <v>14</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B66" s="1">
         <v>1</v>
@@ -3713,10 +3808,10 @@
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -3726,7 +3821,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B67" s="1">
         <v>1</v>
@@ -3738,16 +3833,16 @@
         <v>1</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
@@ -3756,7 +3851,7 @@
     </row>
     <row r="68" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B68" s="1">
         <v>1</v>
@@ -3768,28 +3863,28 @@
         <v>2</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
     <row r="69" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B69" s="1">
         <v>1</v>
@@ -3801,28 +3896,28 @@
         <v>3</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="1:13" ht="57" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B70" s="1">
         <v>1</v>
@@ -3834,28 +3929,30 @@
         <v>4</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="L70" s="1"/>
+        <v>228</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="M70" s="1"/>
     </row>
     <row r="71" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B71" s="1">
         <v>1</v>
@@ -3867,28 +3964,28 @@
         <v>5</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B72" s="1">
         <v>1</v>
@@ -3900,28 +3997,28 @@
         <v>6</v>
       </c>
       <c r="E72" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="H72" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B73" s="1">
         <v>1</v>
@@ -3933,28 +4030,28 @@
         <v>7</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B74" s="1">
         <v>1</v>
@@ -3966,28 +4063,28 @@
         <v>8</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B75" s="1">
         <v>1</v>
@@ -3999,24 +4096,361 @@
         <v>9</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
+    </row>
+    <row r="76" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A76" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1</v>
+      </c>
+      <c r="C76" s="1">
+        <v>6</v>
+      </c>
+      <c r="D76" s="1">
+        <v>10</v>
+      </c>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="L76" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="M76" s="1"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A77" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B77" s="1">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1">
+        <v>6</v>
+      </c>
+      <c r="D77" s="1">
+        <v>11</v>
+      </c>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H77" s="1">
+        <v>5</v>
+      </c>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="L77" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="M77" s="1"/>
+    </row>
+    <row r="78" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A78" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B78" s="1">
+        <v>1</v>
+      </c>
+      <c r="C78" s="1">
+        <v>6</v>
+      </c>
+      <c r="D78" s="1">
+        <v>12</v>
+      </c>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+    </row>
+    <row r="79" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A79" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B79" s="1">
+        <v>1</v>
+      </c>
+      <c r="C79" s="1">
+        <v>6</v>
+      </c>
+      <c r="D79" s="1">
+        <v>13</v>
+      </c>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="L79" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M79" s="1"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A80" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B80" s="1">
+        <v>1</v>
+      </c>
+      <c r="C80" s="1">
+        <v>6</v>
+      </c>
+      <c r="D80" s="1">
+        <v>14</v>
+      </c>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A81" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B81" s="1">
+        <v>1</v>
+      </c>
+      <c r="C81" s="1">
+        <v>7</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1</v>
+      </c>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A82" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B82" s="1">
+        <v>1</v>
+      </c>
+      <c r="C82" s="1">
+        <v>7</v>
+      </c>
+      <c r="D82" s="1">
+        <v>2</v>
+      </c>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+    </row>
+    <row r="83" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A83" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B83" s="1">
+        <v>1</v>
+      </c>
+      <c r="C83" s="1">
+        <v>8</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1</v>
+      </c>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="M83" s="1"/>
+    </row>
+    <row r="84" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A84" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1</v>
+      </c>
+      <c r="C84" s="1">
+        <v>8</v>
+      </c>
+      <c r="D84" s="1">
+        <v>2</v>
+      </c>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="L84" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M84" s="1"/>
+    </row>
+    <row r="85" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A85" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B85" s="1">
+        <v>1</v>
+      </c>
+      <c r="C85" s="1">
+        <v>8</v>
+      </c>
+      <c r="D85" s="1">
+        <v>3</v>
+      </c>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="L85" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="M85" s="1"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A86" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B86" s="1">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1">
+        <v>8</v>
+      </c>
+      <c r="D86" s="1">
+        <v>4</v>
+      </c>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="L86" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="M86" s="1"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A87" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B87" s="1">
+        <v>1</v>
+      </c>
+      <c r="C87" s="1">
+        <v>8</v>
+      </c>
+      <c r="D87" s="1">
+        <v>5</v>
+      </c>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
Add speech sync, wait column, read-only condition handling, and exact command lookup
- Add TTS speech synchronization: runner blocks until client signals speech done
- Add wait column to checklist items for manual confirmation on timeout
- Separate read-only (sim state) vs writable condition handling
- Replace fuzzy command guessing with exact "{label} {status_text}" lookup
- Add checklist load summary with item count and file timestamp
- Skip timeout items instead of blocking when wait is not set
- Update Excel checklist and UI template for new features

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/CopilotAI_Checklists.xlsx
+++ b/CopilotAI_Checklists.xlsx
@@ -8,20 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnl\Documents\projects\CopilotAI\claude_shell_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10000001_{29E35F33-D669-4A3D-A249-8BDE24226DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F464A1F5-59C5-473E-8150-48AE35644544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57840" yWindow="-98" windowWidth="28995" windowHeight="16395" xr2:uid="{B7C423D5-FDD5-4D99-96F7-653924CCE03F}"/>
   </bookViews>
   <sheets>
     <sheet name="ZIBO737" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="179">
   <si>
     <t>checklist</t>
   </si>
@@ -56,57 +68,18 @@
     <t>enabled</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
     <t>PREPUSHBACK</t>
   </si>
   <si>
-    <t>electrical</t>
-  </si>
-  <si>
     <t>item</t>
   </si>
   <si>
     <t>BATTERY</t>
   </si>
   <si>
-    <t>ON and GUARDED</t>
-  </si>
-  <si>
-    <t>APU START</t>
-  </si>
-  <si>
-    <t>APU RUNNING</t>
-  </si>
-  <si>
-    <t>{(sim/cockpit/engine/APU_running:1)&amp;&amp;(laminar/B738/electrical/apu_bus_enable:1)}</t>
-  </si>
-  <si>
-    <t>Long poll - APU takes ~60s</t>
-  </si>
-  <si>
-    <t>APU GENERATORS</t>
-  </si>
-  <si>
     <t>ON</t>
   </si>
   <si>
-    <t>{(sim/cockpit2/electrical/APU_generator_on:1)&amp;&amp;(laminar/B738/annunciator/source_off1:0.0)&amp;&amp;(laminar/B738/annunciator/source_off2:0.0)}</t>
-  </si>
-  <si>
-    <t>GROUND POWER</t>
-  </si>
-  <si>
-    <t>DISCONNECTED</t>
-  </si>
-  <si>
-    <t>laminar/B738/gpu_available:0</t>
-  </si>
-  <si>
-    <t>navigation</t>
-  </si>
-  <si>
     <t>IRS mode selectors</t>
   </si>
   <si>
@@ -116,9 +89,6 @@
     <t>{(laminar/B738/toggle_switch/irs_left:2.0)&amp;&amp;(laminar/B738/toggle_switch/irs_right:2.0}</t>
   </si>
   <si>
-    <t>safety</t>
-  </si>
-  <si>
     <t>EMERGENCY EXIT LIGHTS</t>
   </si>
   <si>
@@ -143,9 +113,6 @@
     <t>laminar/B738/toggle_switch/seatbelt_sign_pos:&gt;0.0</t>
   </si>
   <si>
-    <t>exterior</t>
-  </si>
-  <si>
     <t>Windshield WIPER selectors</t>
   </si>
   <si>
@@ -155,18 +122,6 @@
     <t>sim/cockpit2/switches/wiper_speed:-0.0000</t>
   </si>
   <si>
-    <t>ice_protection</t>
-  </si>
-  <si>
-    <t>WINDOW HEATERS</t>
-  </si>
-  <si>
-    <t>{(laminar/B738/ice/window_heat_l_side_pos:1.0)&amp;&amp;(laminar/B738/ice/window_heat_l_fwd_pos:1.0)&amp;&amp;(laminar/B738/ice/window_heat_r_fwd_pos:1.0)&amp;&amp;(laminar/B738/ice/window_heat_r_side_pos:1.0)}</t>
-  </si>
-  <si>
-    <t>air</t>
-  </si>
-  <si>
     <t>TRIM AIR switch</t>
   </si>
   <si>
@@ -197,9 +152,6 @@
     <t>{(laminar/B738/toggle_switch/bleed_air_apu_pos:1.0)&amp;&amp;(sim/operation/failures/rel_APU_press:0)}</t>
   </si>
   <si>
-    <t>engines</t>
-  </si>
-  <si>
     <t>IGNITION select switch</t>
   </si>
   <si>
@@ -209,9 +161,6 @@
     <t>{(laminar/B738/toggle_switch/eng_start_source:-1)||(laminar/B738/toggle_switch/eng_start_source:1)}</t>
   </si>
   <si>
-    <t>autopilot</t>
-  </si>
-  <si>
     <t>FLIGHT DIRECTORS</t>
   </si>
   <si>
@@ -227,9 +176,6 @@
     <t>laminar/B738/autopilot/disconnect_pos:0.0</t>
   </si>
   <si>
-    <t>instruments</t>
-  </si>
-  <si>
     <t>MODE selector</t>
   </si>
   <si>
@@ -248,9 +194,6 @@
     <t>sim/cockpit/switches/EFIS_shows_weather:0</t>
   </si>
   <si>
-    <t>landing_gear</t>
-  </si>
-  <si>
     <t>LANDING GEAR lever</t>
   </si>
   <si>
@@ -302,36 +245,18 @@
     <t>sim/cockpit/autopilot/airspeed:&gt;140</t>
   </si>
   <si>
-    <t>fuel</t>
-  </si>
-  <si>
-    <t>FUEL PUMPS LEFT and RIGHT</t>
-  </si>
-  <si>
-    <t>{(laminar/B738/fuel/fuel_tank_pos_lft1:1.0)&amp;&amp;(laminar/B738/fuel/fuel_tank_pos_lft2:1.0)&amp;&amp;(sim/operation/failures/rel_ele_fuepmp0:0)&amp;&amp;(laminar/B738/fuel/fuel_tank_pos_rgt1:1.0)&amp;&amp;(laminar/B738/fuel/fuel_tank_pos_rgt2:1.0)&amp;&amp;(sim/operation/failures/rel_ele_fuepmp1:0)}</t>
-  </si>
-  <si>
-    <t>hydraulics</t>
-  </si>
-  <si>
     <t>System B ELECTRIC HYDRAULIC PUMP</t>
   </si>
   <si>
     <t>{(laminar/B738/toggle_switch/electric_hydro_pumps2_pos:1.0)&amp;&amp;(sim/operation/failures/rel_hydpmp_ele:0)}</t>
   </si>
   <si>
-    <t>lights</t>
-  </si>
-  <si>
     <t>ANTI COLLISION LIGHTS</t>
   </si>
   <si>
     <t>{(sim/cockpit/electrical/beacon_lights_on:1)&amp;&amp;(sim/operation/failures/rel_lites_beac:0)}</t>
   </si>
   <si>
-    <t>trim</t>
-  </si>
-  <si>
     <t>AILERON and RUDDER TRIMS</t>
   </si>
   <si>
@@ -341,9 +266,6 @@
     <t>{(sim/cockpit2/controls/aileron_trim:0.0)&amp;&amp;(sim/cockpit2/controls/rudder_trim:0.0)}</t>
   </si>
   <si>
-    <t>doors</t>
-  </si>
-  <si>
     <t>close all Doors</t>
   </si>
   <si>
@@ -359,129 +281,33 @@
     <t>PUSHBACK</t>
   </si>
   <si>
-    <t>ground</t>
-  </si>
-  <si>
     <t>laminar/B738/fms/chock_status:0.0</t>
   </si>
   <si>
-    <t>sim/cockpit2/controls/parking_brake_ratio:0.0</t>
-  </si>
-  <si>
     <t>START_ONE</t>
   </si>
   <si>
     <t>AIR CONDITIONING PACKS</t>
   </si>
   <si>
-    <t>{(laminar/B738/air/l_pack_pos:0.0)&amp;&amp;(laminar/B738/air/r_pack_pos:0.0)}</t>
-  </si>
-  <si>
-    <t>ENGINE 1 START SWITCH</t>
-  </si>
-  <si>
-    <t>GROUND</t>
-  </si>
-  <si>
-    <t>{(laminar/B738/engine/starter1_pos:0)&amp;&amp;(sim/operation/failures/rel_startr0:0)}</t>
-  </si>
-  <si>
-    <t>N2 REACHING 25%</t>
-  </si>
-  <si>
-    <t>check</t>
-  </si>
-  <si>
     <t>laminar/B738/engine/indicators/N2_percent_1:&gt;22</t>
   </si>
   <si>
-    <t>ENGINE 1 START LEVER</t>
-  </si>
-  <si>
-    <t>IDLE</t>
-  </si>
-  <si>
-    <t>laminar/B738/engine/mixture_ratio1:1.0</t>
-  </si>
-  <si>
-    <t>ENGINE 1</t>
-  </si>
-  <si>
-    <t>STABLE IDLE</t>
-  </si>
-  <si>
     <t>START_TWO</t>
   </si>
   <si>
-    <t>ENGINE 2 START switch</t>
-  </si>
-  <si>
-    <t>{(laminar/B738/engine/starter2_pos:0)&amp;&amp;(sim/operation/failures/rel_startr1:0)}</t>
-  </si>
-  <si>
     <t>laminar/B738/engine/indicators/N2_percent_2:&gt;22</t>
   </si>
   <si>
-    <t>ENGINE 2 START LEVER</t>
-  </si>
-  <si>
-    <t>laminar/B738/engine/mixture_ratio2:1.0</t>
-  </si>
-  <si>
-    <t>ENGINE 2</t>
-  </si>
-  <si>
-    <t>System A ELECTRIC HYDRAULIC PUMP</t>
-  </si>
-  <si>
-    <t>{(laminar/B738/toggle_switch/electric_hydro_pumps1_pos:1.0)&amp;&amp;(sim/operation/failures/rel_hydpmp_ele:0)}</t>
-  </si>
-  <si>
-    <t>{(sim/cockpit2/electrical/generator_on[0]:1.0)&amp;&amp;(sim/operation/failures/rel_genera0:0)&amp;&amp;(sim/cockpit2/electrical/generator_on[1]:1.0)&amp;&amp;(sim/operation/failures/rel_genera1:0)}</t>
-  </si>
-  <si>
-    <t>BRAKE</t>
-  </si>
-  <si>
     <t>UNBLOCK</t>
   </si>
   <si>
-    <t>GENERATOR</t>
-  </si>
-  <si>
     <t>PREFLIGHT</t>
   </si>
   <si>
     <t>cmd:axp/commands/autoclose_all_doors</t>
   </si>
   <si>
-    <t>Forward Left Door</t>
-  </si>
-  <si>
-    <t>Close Doors</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>Forward Right Door</t>
-  </si>
-  <si>
-    <t>Forward Cargo Door</t>
-  </si>
-  <si>
-    <t>Aft Cargo Door</t>
-  </si>
-  <si>
-    <t>Aft Right Door</t>
-  </si>
-  <si>
-    <t>Aft Left Door</t>
-  </si>
-  <si>
     <t>cmd:laminar/B738/door/fwd_L_toggle</t>
   </si>
   <si>
@@ -503,96 +329,30 @@
     <t>cmd:laminar/B738/push_button/flt_dk_door_open</t>
   </si>
   <si>
-    <t>Cockpit Deck Door</t>
-  </si>
-  <si>
-    <t>BLOCK</t>
-  </si>
-  <si>
-    <t>WHEELS</t>
-  </si>
-  <si>
-    <t>power</t>
-  </si>
-  <si>
-    <t>brakes</t>
-  </si>
-  <si>
-    <t>chocks</t>
-  </si>
-  <si>
-    <t>GPU</t>
-  </si>
-  <si>
-    <t>CONNECT</t>
-  </si>
-  <si>
-    <t>WHITE_DOME_LIGHT</t>
-  </si>
-  <si>
     <t>cmd:laminar/B738/toggle_switch/gpu_dn</t>
   </si>
   <si>
     <t>cmd:laminar/B738/toggle_switch/cockpit_dome_dn</t>
   </si>
   <si>
-    <t>link</t>
-  </si>
-  <si>
-    <t>cmd:laminar/B738/toggle_switch/gpu_up</t>
-  </si>
-  <si>
-    <t>DISCONNECT</t>
-  </si>
-  <si>
-    <t>EXTERNAL POWER</t>
-  </si>
-  <si>
-    <t>group2</t>
-  </si>
-  <si>
     <t>PRETAXI</t>
   </si>
   <si>
-    <t>brake</t>
-  </si>
-  <si>
-    <t>(laminar/B738/toggle_switch/electric_hydro_pumps1_pos:1.0)&amp;&amp;(sim/operation/failures/rel_hydpmp_ele:0)</t>
-  </si>
-  <si>
-    <t>pump</t>
-  </si>
-  <si>
-    <t>laminar/B738/engine/indicators/N2_percent_1:&gt;55</t>
-  </si>
-  <si>
-    <t>laminar/B738/engine/indicators/N2_percent_2:&gt;55</t>
-  </si>
-  <si>
     <t>(sim/cockpit2/electrical/generator_on[0]:1.0)&amp;&amp;(sim/operation/failures/rel_genera0:0)&amp;&amp;(sim/cockpit2/electrical/generator_on[1]:1.0)&amp;&amp;(sim/operation/failures/rel_genera1:0)</t>
   </si>
   <si>
     <t>ENGINE GENERATORS</t>
   </si>
   <si>
-    <t>generators</t>
-  </si>
-  <si>
     <t>PROBE HEAT SWITCHES</t>
   </si>
   <si>
-    <t>probe heat</t>
-  </si>
-  <si>
     <t>(laminar/B738/air/l_pack_pos:1.0)&amp;&amp;(laminar/B738/air/r_pack_pos:1.0)</t>
   </si>
   <si>
     <t>AIR CONDITIONING PACK SWITCHES</t>
   </si>
   <si>
-    <t>A/C</t>
-  </si>
-  <si>
     <t>laminar/B738/air/isolation_valve_pos:1.0</t>
   </si>
   <si>
@@ -617,12 +377,6 @@
     <t>APU SWITCH</t>
   </si>
   <si>
-    <t>pressure</t>
-  </si>
-  <si>
-    <t>APU</t>
-  </si>
-  <si>
     <t>CONTINUOUS</t>
   </si>
   <si>
@@ -641,9 +395,6 @@
     <t>ENGINE START</t>
   </si>
   <si>
-    <t>cmdhold:0.5:laminar/B738/rotary/eng1_start_cont; cmdhold:laminar/B738/rotary/eng2_start_cont;</t>
-  </si>
-  <si>
     <t>toggle:laminar/B738/toggle_switch/yaw_dumper=laminar/B738/toggle_switch/yaw_dumper_pos:1;</t>
   </si>
   <si>
@@ -683,27 +434,12 @@
     <t>cmd:laminar/B738/knob/transponder_tara</t>
   </si>
   <si>
-    <t>set:laminar/B738/fms/chock_status=1;</t>
-  </si>
-  <si>
-    <t>cmd:laminar/B738/push_button/park_brake_on_off</t>
-  </si>
-  <si>
-    <t>laminar/B738/annunciator/parking_brake:&gt;0.01</t>
-  </si>
-  <si>
     <t>cmd:laminar/B738/gpu_toggle</t>
   </si>
   <si>
     <t>laminar/B738/gpu_available:1.0</t>
   </si>
   <si>
-    <t>cmd:laminar/B738/button_switch_cover02</t>
-  </si>
-  <si>
-    <t>laminar/B738/button_switch/cover_position[2]:0</t>
-  </si>
-  <si>
     <t>set:laminar/B738/toggle_switch/capt_probes_pos=1; set:laminar/B738/toggle_switch/fo_probes_pos=1;</t>
   </si>
   <si>
@@ -711,6 +447,129 @@
   </si>
   <si>
     <t>set:laminar/B738/switch/land_lights_left_pos=1; set:laminar/B738/switch/land_lights_right_pos=1;</t>
+  </si>
+  <si>
+    <t>Remove chocks</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/engine/mixture1_idle</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/engine/mixture2_idle</t>
+  </si>
+  <si>
+    <t>laminar/B738/engine/indicators/N2_percent_2:&gt;50</t>
+  </si>
+  <si>
+    <t>Spooling</t>
+  </si>
+  <si>
+    <t>START TWO</t>
+  </si>
+  <si>
+    <t>START ONE</t>
+  </si>
+  <si>
+    <t>laminar/B738/engine/indicators/N2_percent_1:&gt;50</t>
+  </si>
+  <si>
+    <t>N2 is greater than 22%, set Mixture to Idle</t>
+  </si>
+  <si>
+    <t>N2 is greater than 50%, Start Complete</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/rotary/eng2_start_off;</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/rotary/eng1_start_off;</t>
+  </si>
+  <si>
+    <t>cmdhold:0.1:laminar/B738/rotary/eng1_start_cont; cmdhold:0.1:laminar/B738/rotary/eng2_start_cont;</t>
+  </si>
+  <si>
+    <t>GPU  Disconnect</t>
+  </si>
+  <si>
+    <t>Battery On</t>
+  </si>
+  <si>
+    <t>Brake On</t>
+  </si>
+  <si>
+    <t>Start APU</t>
+  </si>
+  <si>
+    <t>APU Online</t>
+  </si>
+  <si>
+    <t>FUEL_PUMP</t>
+  </si>
+  <si>
+    <t>cmd.setDataRefValue("laminar/B738/fuel/fuel_tank_pos_lft1", 1);</t>
+  </si>
+  <si>
+    <t>cmd.setDataRefValue("laminar/B738/fuel/fuel_tank_pos_lft2", 1);</t>
+  </si>
+  <si>
+    <t>cmd.setDataRefValue("laminar/B738/fuel/fuel_tank_pos_ctr1", 1);</t>
+  </si>
+  <si>
+    <t>cmd.setDataRefValue("laminar/B738/fuel/fuel_tank_pos_ctr2", 1);</t>
+  </si>
+  <si>
+    <t>cmd.setDataRefValue("laminar/B738/fuel/fuel_tank_pos_rgt1", 1);</t>
+  </si>
+  <si>
+    <t>cmd.setDataRefValue("laminar/B738/fuel/fuel_tank_pos_rgt2", 1);</t>
+  </si>
+  <si>
+    <t>laminar/B738/electrical/apu_bus_enable:1</t>
+  </si>
+  <si>
+    <t>cmdhold:1.0:laminar/B738/toggle_switch/apu_gen1_dn; cmdhold:1.0:laminar/B738/toggle_switch/apu_gen2_dn;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmd:laminar/B738/toggle_switch/window_heat_l_fwd; cmd:laminar/B738/toggle_switch/window_heat_l_side; cmd:laminar/B738/toggle_switch/window_heat_r_fwd; cmd:laminar/B738/toggle_switch/window_heat_r_side; </t>
+  </si>
+  <si>
+    <t>Window Heat ON</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/fms/chock_status</t>
+  </si>
+  <si>
+    <t>Chock  Wheels</t>
+  </si>
+  <si>
+    <t>Open Exterior Doors and Hatches</t>
+  </si>
+  <si>
+    <t>Illuminate Cockpit</t>
+  </si>
+  <si>
+    <t>Connect Ground Power Unit</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>cmdhold:2.0:laminar/B738/spring_toggle_switch/APU_start_pos_dn; cmd:laminar/B738/spring_toggle_switch/APU_start_pos_dn;</t>
+  </si>
+  <si>
+    <t>laminar/B738/fmod/gpu_deployed:1</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/rotary/eng2_start_off; cmd:laminar/B738/rotary/eng1_start_grd; cmd:laminar/B738/engine/mixture1_cutoff;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAKE </t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/rotary/eng1_start_off; cmd:laminar/B738/rotary/eng2_start_grd; cmd:laminar/B738/engine/mixture2_cutoff;</t>
+  </si>
+  <si>
+    <t>Fuel Pumps On and On and On</t>
   </si>
 </sst>
 </file>
@@ -1250,10 +1109,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1310,22 +1166,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}" name="ZIBO737" displayName="ZIBO737" ref="A1:M87" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:M87" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D7EB0E30-B8BB-40E3-B6DB-C78633A8AE10}" name="checklist" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{3F7C8B58-5F6F-4EDC-93DE-0EFE3A81396D}" name="enabled" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{01D1E4D6-1DB5-47B3-AAB3-A1B68150B44F}" name="group" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{72FFAAE9-5D8C-40EB-AE40-8F469B0E7D59}" name="order" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{920337F0-56EA-4F1F-986B-102213412169}" name="group2" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}" name="ZIBO737" displayName="ZIBO737" ref="A1:L87" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L87" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L87">
+    <sortCondition ref="C1:C87"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{D7EB0E30-B8BB-40E3-B6DB-C78633A8AE10}" name="checklist" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{3F7C8B58-5F6F-4EDC-93DE-0EFE3A81396D}" name="enabled" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{01D1E4D6-1DB5-47B3-AAB3-A1B68150B44F}" name="group" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{72FFAAE9-5D8C-40EB-AE40-8F469B0E7D59}" name="order" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{36676C6C-49EA-4FF9-8E63-6BEF44843C00}" name="type" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{460E5C61-EEC5-4F96-9F6B-BAE749518F16}" name="label" dataDxfId="6"/>
     <tableColumn id="6" xr3:uid="{197D6612-0EC9-4731-A70B-559CA562709F}" name="status_text" dataDxfId="5"/>
     <tableColumn id="7" xr3:uid="{077D9AF1-4A41-4A35-8CA8-A7F43BA57B29}" name="speak" dataDxfId="4"/>
     <tableColumn id="8" xr3:uid="{BF0DE601-6A90-4914-943B-FB3758618C69}" name="speak_on" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{58980946-BD94-4B4D-B114-12165AE8D78E}" name="conditions" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{6283B833-A799-4A62-B487-95ED808B28CD}" name="commands" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{E1F6A41E-D7AD-4672-B6E5-6DABB0756EF2}" name="notes" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{F3AA39CB-4F4D-4AFB-96FA-D0E6FF38E2D5}" name="wait" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{58980946-BD94-4B4D-B114-12165AE8D78E}" name="conditions" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{6283B833-A799-4A62-B487-95ED808B28CD}" name="commands" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1651,8 +1509,8 @@
   <dimension ref="A1:N87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L77" sqref="L77"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1661,19 +1519,18 @@
     <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.19921875" customWidth="1"/>
     <col min="4" max="4" width="9.06640625" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.46484375" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.796875" customWidth="1"/>
+    <col min="9" max="9" width="10.46484375" customWidth="1"/>
+    <col min="10" max="10" width="6.46484375" customWidth="1"/>
     <col min="11" max="11" width="49.1328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="41.265625" customWidth="1"/>
-    <col min="13" max="13" width="13.796875" customWidth="1"/>
-    <col min="14" max="14" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.46484375" customWidth="1"/>
+    <col min="13" max="13" width="21.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1687,22 +1544,22 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>175</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>172</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1710,13 +1567,10 @@
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1728,27 +1582,24 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>145</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" s="1"/>
+        <v>169</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -1760,27 +1611,22 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I3" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -1792,27 +1638,22 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I4" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1824,27 +1665,22 @@
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I5" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -1856,27 +1692,22 @@
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I6" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1888,27 +1719,22 @@
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I7" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -1920,27 +1746,22 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I8" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="L8" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1952,27 +1773,22 @@
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I9" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -1984,27 +1800,27 @@
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>161</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I10" s="1"/>
+        <v>168</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
       <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="L10" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2016,30 +1832,27 @@
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>166</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I11" s="1"/>
+        <v>171</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>224</v>
+        <v>134</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -2051,27 +1864,22 @@
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="L12" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -2083,27 +1891,22 @@
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -2115,27 +1918,24 @@
         <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>168</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="1"/>
+        <v>170</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -2147,23 +1947,22 @@
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>171</v>
+        <v>80</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -2175,30 +1974,26 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -2210,33 +2005,29 @@
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>164</v>
+        <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="H17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" ht="57" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -2245,33 +2036,27 @@
         <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
       <c r="J18" s="1"/>
-      <c r="K18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="L18" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -2280,31 +2065,32 @@
         <v>4</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+        <v>155</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
       <c r="K19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+        <v>163</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -2313,718 +2099,696 @@
         <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
       <c r="L20" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
       </c>
       <c r="D21" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>163</v>
+        <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="I21" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
       <c r="J21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
       </c>
       <c r="D23" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I23" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
       </c>
       <c r="D24" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:12" ht="57" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
       </c>
       <c r="D26" s="1">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="L26" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="B27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
       </c>
       <c r="D27" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
       </c>
       <c r="D28" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
       </c>
       <c r="D29" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
       </c>
       <c r="D30" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
       </c>
       <c r="D31" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I31" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
       </c>
       <c r="D32" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1">
+        <v>1</v>
+      </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
       </c>
       <c r="D33" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I33" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1">
+        <v>1</v>
+      </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-    </row>
-    <row r="34" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="1">
         <v>2</v>
       </c>
       <c r="D34" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1">
+        <v>1</v>
+      </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="1">
         <v>2</v>
       </c>
       <c r="D35" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I35" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1">
+        <v>1</v>
+      </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" s="1">
         <v>2</v>
       </c>
       <c r="D36" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I36" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1">
+        <v>1</v>
+      </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" s="1">
         <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I37" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1">
+        <v>1</v>
+      </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
       </c>
       <c r="D38" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I38" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1">
+        <v>1</v>
+      </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-    </row>
-    <row r="39" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
       </c>
       <c r="D39" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I39" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1">
+        <v>1</v>
+      </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="40" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="1">
         <v>2</v>
       </c>
       <c r="D40" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I40" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1">
+        <v>1</v>
+      </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" s="1">
         <v>2</v>
       </c>
       <c r="D41" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I41" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1">
+        <v>1</v>
+      </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-    </row>
-    <row r="42" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -3033,31 +2797,32 @@
         <v>2</v>
       </c>
       <c r="D42" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="H42" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I42" s="1"/>
+        <v>178</v>
+      </c>
+      <c r="I42" s="1">
+        <v>1</v>
+      </c>
       <c r="J42" s="1"/>
-      <c r="K42" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N42" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43" s="1">
         <v>1</v>
@@ -3066,31 +2831,33 @@
         <v>2</v>
       </c>
       <c r="D43" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1">
+        <v>1</v>
+      </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-    </row>
-    <row r="44" spans="1:13" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="N43" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -3099,31 +2866,33 @@
         <v>2</v>
       </c>
       <c r="D44" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1">
+        <v>1</v>
+      </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-    </row>
-    <row r="45" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="N44" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
@@ -3132,31 +2901,33 @@
         <v>2</v>
       </c>
       <c r="D45" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I45" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1">
+        <v>1</v>
+      </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-    </row>
-    <row r="46" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="N45" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46" s="1">
         <v>1</v>
@@ -3165,31 +2936,33 @@
         <v>2</v>
       </c>
       <c r="D46" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I46" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1">
+        <v>1</v>
+      </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-    </row>
-    <row r="47" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="N46" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -3198,90 +2971,58 @@
         <v>2</v>
       </c>
       <c r="D47" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I47" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1">
+        <v>1</v>
+      </c>
       <c r="J47" s="1"/>
-      <c r="K47" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-    </row>
-    <row r="48" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A48" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="N47" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A48" s="1"/>
       <c r="B48" s="1">
         <v>1</v>
       </c>
-      <c r="C48" s="1">
-        <v>2</v>
-      </c>
-      <c r="D48" s="1">
-        <v>33</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>108</v>
-      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A49" s="1" t="s">
-        <v>12</v>
-      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A49" s="1"/>
       <c r="B49" s="1">
         <v>1</v>
       </c>
-      <c r="C49" s="1">
-        <v>2</v>
-      </c>
-      <c r="D49" s="1">
-        <v>34</v>
-      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -3293,28 +3034,29 @@
         <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I50" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="I50" s="1">
+        <v>1</v>
+      </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="B51" s="1">
         <v>1</v>
@@ -3326,87 +3068,52 @@
         <v>2</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I51" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1">
+        <v>1</v>
+      </c>
       <c r="J51" s="1"/>
-      <c r="K51" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A52" s="1" t="s">
-        <v>111</v>
-      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A52" s="1"/>
       <c r="B52" s="1">
         <v>1</v>
       </c>
-      <c r="C52" s="1">
-        <v>3</v>
-      </c>
-      <c r="D52" s="1">
-        <v>3</v>
-      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>115</v>
-      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-    </row>
-    <row r="53" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A53" s="1" t="s">
-        <v>115</v>
-      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A53" s="1"/>
       <c r="B53" s="1">
         <v>1</v>
       </c>
-      <c r="C53" s="1">
-        <v>4</v>
-      </c>
-      <c r="D53" s="1">
-        <v>1</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
-      <c r="K53" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-    </row>
-    <row r="54" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="B54" s="1">
         <v>1</v>
@@ -3415,31 +3122,27 @@
         <v>4</v>
       </c>
       <c r="D54" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I54" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1">
+        <v>1</v>
+      </c>
       <c r="J54" s="1"/>
-      <c r="K54" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="55" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="B55" s="1">
         <v>1</v>
@@ -3448,31 +3151,27 @@
         <v>4</v>
       </c>
       <c r="D55" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
       <c r="H55" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I55" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="I55" s="1">
+        <v>1</v>
+      </c>
       <c r="J55" s="1"/>
-      <c r="K55" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L55" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="B56" s="1">
         <v>1</v>
@@ -3481,31 +3180,25 @@
         <v>4</v>
       </c>
       <c r="D56" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
       <c r="H56" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I56" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="I56" s="1">
+        <v>1</v>
+      </c>
       <c r="J56" s="1"/>
-      <c r="K56" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="57" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
@@ -3514,31 +3207,30 @@
         <v>4</v>
       </c>
       <c r="D57" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>127</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
       <c r="H57" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I57" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="I57" s="1">
+        <v>1</v>
+      </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="B58" s="1">
         <v>1</v>
@@ -3547,123 +3239,87 @@
         <v>4</v>
       </c>
       <c r="D58" s="1">
+        <v>5</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I58" s="1">
+        <v>1</v>
+      </c>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A59" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1">
+        <v>4</v>
+      </c>
+      <c r="D59" s="1">
         <v>6</v>
       </c>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-    </row>
-    <row r="59" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A59" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B59" s="1">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1">
-        <v>5</v>
-      </c>
-      <c r="D59" s="1">
-        <v>1</v>
-      </c>
       <c r="E59" s="1" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I59" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1">
+        <v>1</v>
+      </c>
       <c r="J59" s="1"/>
-      <c r="K59" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-    </row>
-    <row r="60" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A60" s="1" t="s">
-        <v>129</v>
-      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A60" s="1"/>
       <c r="B60" s="1">
         <v>1</v>
       </c>
-      <c r="C60" s="1">
-        <v>5</v>
-      </c>
-      <c r="D60" s="1">
-        <v>2</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A61" s="1" t="s">
-        <v>129</v>
-      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A61" s="1"/>
       <c r="B61" s="1">
         <v>1</v>
       </c>
-      <c r="C61" s="1">
-        <v>5</v>
-      </c>
-      <c r="D61" s="1">
-        <v>3</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="B62" s="1">
         <v>1</v>
@@ -3672,31 +3328,27 @@
         <v>5</v>
       </c>
       <c r="D62" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I62" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1">
+        <v>1</v>
+      </c>
       <c r="J62" s="1"/>
-      <c r="K62" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="63" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="B63" s="1">
         <v>1</v>
@@ -3705,31 +3357,27 @@
         <v>5</v>
       </c>
       <c r="D63" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>135</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
       <c r="H63" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I63" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="I63" s="1">
+        <v>1</v>
+      </c>
       <c r="J63" s="1"/>
-      <c r="K63" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-    </row>
-    <row r="64" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="L63" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
@@ -3738,31 +3386,25 @@
         <v>5</v>
       </c>
       <c r="D64" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>136</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
       <c r="H64" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I64" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="I64" s="1">
+        <v>1</v>
+      </c>
       <c r="J64" s="1"/>
-      <c r="K64" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-    </row>
-    <row r="65" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="65" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="B65" s="1">
         <v>1</v>
@@ -3771,31 +3413,30 @@
         <v>5</v>
       </c>
       <c r="D65" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>141</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
       <c r="H65" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I65" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="I65" s="1">
+        <v>1</v>
+      </c>
       <c r="J65" s="1"/>
       <c r="K65" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="B66" s="1">
         <v>1</v>
@@ -3804,120 +3445,87 @@
         <v>5</v>
       </c>
       <c r="D66" s="1">
-        <v>8</v>
-      </c>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I66" s="1">
+        <v>1</v>
+      </c>
       <c r="J66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="K66" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>176</v>
+        <v>86</v>
       </c>
       <c r="B67" s="1">
         <v>1</v>
       </c>
       <c r="C67" s="1">
+        <v>5</v>
+      </c>
+      <c r="D67" s="1">
         <v>6</v>
       </c>
-      <c r="D67" s="1">
-        <v>1</v>
-      </c>
       <c r="E67" s="1" t="s">
-        <v>177</v>
+        <v>80</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I67" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1">
+        <v>1</v>
+      </c>
       <c r="J67" s="1"/>
       <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-    </row>
-    <row r="68" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A68" s="1" t="s">
-        <v>176</v>
-      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A68" s="1"/>
       <c r="B68" s="1">
         <v>1</v>
       </c>
-      <c r="C68" s="1">
-        <v>6</v>
-      </c>
-      <c r="D68" s="1">
-        <v>2</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
-      <c r="K68" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-    </row>
-    <row r="69" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A69" s="1" t="s">
-        <v>176</v>
-      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A69" s="1"/>
       <c r="B69" s="1">
         <v>1</v>
       </c>
-      <c r="C69" s="1">
-        <v>6</v>
-      </c>
-      <c r="D69" s="1">
-        <v>3</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
-      <c r="K69" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-    </row>
-    <row r="70" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="70" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B70" s="1">
         <v>1</v>
@@ -3926,33 +3534,30 @@
         <v>6</v>
       </c>
       <c r="D70" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="F70" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G70" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G70" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1">
+        <v>1</v>
+      </c>
       <c r="J70" s="1"/>
       <c r="K70" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="L70" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="M70" s="1"/>
-    </row>
-    <row r="71" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+        <v>101</v>
+      </c>
+      <c r="L70" s="1"/>
+    </row>
+    <row r="71" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B71" s="1">
         <v>1</v>
@@ -3961,31 +3566,32 @@
         <v>6</v>
       </c>
       <c r="D71" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>189</v>
+        <v>12</v>
       </c>
       <c r="F71" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G71" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1">
+        <v>1</v>
+      </c>
       <c r="J71" s="1"/>
       <c r="K71" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
+        <v>136</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B72" s="1">
         <v>1</v>
@@ -3994,31 +3600,30 @@
         <v>6</v>
       </c>
       <c r="D72" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>189</v>
+        <v>12</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I72" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1">
+        <v>1</v>
+      </c>
       <c r="J72" s="1"/>
       <c r="K72" s="1" t="s">
-        <v>190</v>
+        <v>104</v>
       </c>
       <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B73" s="1">
         <v>1</v>
@@ -4027,31 +3632,30 @@
         <v>6</v>
       </c>
       <c r="D73" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>198</v>
+        <v>12</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I73" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1">
+        <v>1</v>
+      </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1" t="s">
-        <v>192</v>
+        <v>106</v>
       </c>
       <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B74" s="1">
         <v>1</v>
@@ -4060,31 +3664,30 @@
         <v>6</v>
       </c>
       <c r="D74" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>199</v>
+        <v>12</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I74" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1">
+        <v>1</v>
+      </c>
       <c r="J74" s="1"/>
       <c r="K74" s="1" t="s">
-        <v>194</v>
+        <v>108</v>
       </c>
       <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B75" s="1">
         <v>1</v>
@@ -4093,31 +3696,30 @@
         <v>6</v>
       </c>
       <c r="D75" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>199</v>
+        <v>12</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I75" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1">
+        <v>1</v>
+      </c>
       <c r="J75" s="1"/>
       <c r="K75" s="1" t="s">
-        <v>196</v>
+        <v>110</v>
       </c>
       <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
-    </row>
-    <row r="76" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B76" s="1">
         <v>1</v>
@@ -4126,28 +3728,30 @@
         <v>6</v>
       </c>
       <c r="D76" s="1">
-        <v>10</v>
-      </c>
-      <c r="E76" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F76" s="1" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I76" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1">
+        <v>1</v>
+      </c>
       <c r="J76" s="1"/>
-      <c r="L76" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="M76" s="1"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="K76" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L76" s="1"/>
+    </row>
+    <row r="77" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B77" s="1">
         <v>1</v>
@@ -4156,28 +3760,29 @@
         <v>6</v>
       </c>
       <c r="D77" s="1">
-        <v>11</v>
-      </c>
-      <c r="E77" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F77" s="1" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="H77" s="1">
-        <v>5</v>
-      </c>
-      <c r="I77" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1">
+        <v>1</v>
+      </c>
       <c r="J77" s="1"/>
       <c r="L77" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="M77" s="1"/>
-    </row>
-    <row r="78" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B78" s="1">
         <v>1</v>
@@ -4186,29 +3791,29 @@
         <v>6</v>
       </c>
       <c r="D78" s="1">
-        <v>12</v>
-      </c>
-      <c r="E78" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F78" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I78" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="G78" s="1">
+        <v>5</v>
+      </c>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1">
+        <v>1</v>
+      </c>
       <c r="J78" s="1"/>
-      <c r="K78" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="L78" s="1"/>
-      <c r="M78" s="1"/>
-    </row>
-    <row r="79" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="L78" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B79" s="1">
         <v>1</v>
@@ -4217,28 +3822,30 @@
         <v>6</v>
       </c>
       <c r="D79" s="1">
-        <v>13</v>
-      </c>
-      <c r="E79" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F79" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G79" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1">
+        <v>1</v>
+      </c>
       <c r="J79" s="1"/>
-      <c r="L79" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="M79" s="1"/>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="K79" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L79" s="1"/>
+    </row>
+    <row r="80" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B80" s="1">
         <v>1</v>
@@ -4247,48 +3854,56 @@
         <v>6</v>
       </c>
       <c r="D80" s="1">
+        <v>11</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G80" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
+      <c r="I80" s="1">
+        <v>1</v>
+      </c>
       <c r="J80" s="1"/>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L80" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>209</v>
+        <v>100</v>
       </c>
       <c r="B81" s="1">
         <v>1</v>
       </c>
       <c r="C81" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D81" s="1">
-        <v>1</v>
-      </c>
-      <c r="E81" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="F81" s="1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
+      <c r="I81" s="1">
+        <v>1</v>
+      </c>
       <c r="J81" s="1"/>
       <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
-        <v>209</v>
+        <v>122</v>
       </c>
       <c r="B82" s="1">
         <v>1</v>
@@ -4297,55 +3912,50 @@
         <v>7</v>
       </c>
       <c r="D82" s="1">
-        <v>2</v>
-      </c>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>210</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
       <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
+      <c r="I82" s="1">
+        <v>1</v>
+      </c>
       <c r="J82" s="1"/>
       <c r="L82" s="1"/>
-      <c r="M82" s="1"/>
-    </row>
-    <row r="83" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
-        <v>210</v>
+        <v>122</v>
       </c>
       <c r="B83" s="1">
         <v>1</v>
       </c>
       <c r="C83" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D83" s="1">
-        <v>1</v>
-      </c>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I83" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1">
+        <v>1</v>
+      </c>
       <c r="J83" s="1"/>
-      <c r="K83" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="M83" s="1"/>
-    </row>
-    <row r="84" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="L83" s="1"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
-        <v>210</v>
+        <v>123</v>
       </c>
       <c r="B84" s="1">
         <v>1</v>
@@ -4354,26 +3964,32 @@
         <v>8</v>
       </c>
       <c r="D84" s="1">
-        <v>2</v>
-      </c>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G84" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I84" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1">
+        <v>1</v>
+      </c>
       <c r="J84" s="1"/>
+      <c r="K84" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="L84" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="M84" s="1"/>
-    </row>
-    <row r="85" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>210</v>
+        <v>123</v>
       </c>
       <c r="B85" s="1">
         <v>1</v>
@@ -4382,26 +3998,29 @@
         <v>8</v>
       </c>
       <c r="D85" s="1">
-        <v>3</v>
-      </c>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="G85" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="I85" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1">
+        <v>1</v>
+      </c>
       <c r="J85" s="1"/>
       <c r="L85" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="M85" s="1"/>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>210</v>
+        <v>123</v>
       </c>
       <c r="B86" s="1">
         <v>1</v>
@@ -4410,29 +4029,29 @@
         <v>8</v>
       </c>
       <c r="D86" s="1">
-        <v>4</v>
-      </c>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="G86" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="I86" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1">
+        <v>1</v>
+      </c>
       <c r="J86" s="1"/>
-      <c r="K86" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="L86" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="M86" s="1"/>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
-        <v>210</v>
+        <v>123</v>
       </c>
       <c r="B87" s="1">
         <v>1</v>
@@ -4441,16 +4060,28 @@
         <v>8</v>
       </c>
       <c r="D87" s="1">
-        <v>5</v>
-      </c>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
+      <c r="I87" s="1">
+        <v>1</v>
+      </c>
       <c r="J87" s="1"/>
-      <c r="L87" s="1"/>
-      <c r="M87" s="1"/>
+      <c r="K87" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L87" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
Update CopilotAI checklists spreadsheet
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/CopilotAI_Checklists.xlsx
+++ b/CopilotAI_Checklists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnl\Documents\projects\CopilotAI\claude_shell_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F464A1F5-59C5-473E-8150-48AE35644544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5926E4-ACAC-432A-A8ED-FA2C45841F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57840" yWindow="-98" windowWidth="28995" windowHeight="16395" xr2:uid="{B7C423D5-FDD5-4D99-96F7-653924CCE03F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="194">
   <si>
     <t>checklist</t>
   </si>
@@ -80,9 +80,6 @@
     <t>ON</t>
   </si>
   <si>
-    <t>IRS mode selectors</t>
-  </si>
-  <si>
     <t>NAV</t>
   </si>
   <si>
@@ -245,33 +242,12 @@
     <t>sim/cockpit/autopilot/airspeed:&gt;140</t>
   </si>
   <si>
-    <t>System B ELECTRIC HYDRAULIC PUMP</t>
-  </si>
-  <si>
-    <t>{(laminar/B738/toggle_switch/electric_hydro_pumps2_pos:1.0)&amp;&amp;(sim/operation/failures/rel_hydpmp_ele:0)}</t>
-  </si>
-  <si>
-    <t>ANTI COLLISION LIGHTS</t>
-  </si>
-  <si>
     <t>{(sim/cockpit/electrical/beacon_lights_on:1)&amp;&amp;(sim/operation/failures/rel_lites_beac:0)}</t>
   </si>
   <si>
-    <t>AILERON and RUDDER TRIMS</t>
-  </si>
-  <si>
-    <t>CHECK 0</t>
-  </si>
-  <si>
     <t>{(sim/cockpit2/controls/aileron_trim:0.0)&amp;&amp;(sim/cockpit2/controls/rudder_trim:0.0)}</t>
   </si>
   <si>
-    <t>close all Doors</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
     <t>{(737u/doors/L1:0)&amp;&amp;(737u/doors/R1:0)&amp;&amp;(737u/doors/R2:0)&amp;&amp;(737u/doors/Fwd_Cargo:0)&amp;&amp;(737u/doors/aft_Cargo:0)}</t>
   </si>
   <si>
@@ -302,6 +278,9 @@
     <t>UNBLOCK</t>
   </si>
   <si>
+    <t>GENERATOR</t>
+  </si>
+  <si>
     <t>PREFLIGHT</t>
   </si>
   <si>
@@ -329,30 +308,12 @@
     <t>cmd:laminar/B738/push_button/flt_dk_door_open</t>
   </si>
   <si>
-    <t>cmd:laminar/B738/toggle_switch/gpu_dn</t>
-  </si>
-  <si>
-    <t>cmd:laminar/B738/toggle_switch/cockpit_dome_dn</t>
-  </si>
-  <si>
     <t>PRETAXI</t>
   </si>
   <si>
-    <t>(sim/cockpit2/electrical/generator_on[0]:1.0)&amp;&amp;(sim/operation/failures/rel_genera0:0)&amp;&amp;(sim/cockpit2/electrical/generator_on[1]:1.0)&amp;&amp;(sim/operation/failures/rel_genera1:0)</t>
-  </si>
-  <si>
-    <t>ENGINE GENERATORS</t>
-  </si>
-  <si>
-    <t>PROBE HEAT SWITCHES</t>
-  </si>
-  <si>
     <t>(laminar/B738/air/l_pack_pos:1.0)&amp;&amp;(laminar/B738/air/r_pack_pos:1.0)</t>
   </si>
   <si>
-    <t>AIR CONDITIONING PACK SWITCHES</t>
-  </si>
-  <si>
     <t>laminar/B738/air/isolation_valve_pos:1.0</t>
   </si>
   <si>
@@ -377,9 +338,6 @@
     <t>APU SWITCH</t>
   </si>
   <si>
-    <t>CONTINUOUS</t>
-  </si>
-  <si>
     <t>FLAPS</t>
   </si>
   <si>
@@ -392,15 +350,6 @@
     <t>YAW DAMPER</t>
   </si>
   <si>
-    <t>ENGINE START</t>
-  </si>
-  <si>
-    <t>toggle:laminar/B738/toggle_switch/yaw_dumper=laminar/B738/toggle_switch/yaw_dumper_pos:1;</t>
-  </si>
-  <si>
-    <t>cmd:laminar/B738/push_button/flaps_5</t>
-  </si>
-  <si>
     <t>TAXI</t>
   </si>
   <si>
@@ -434,15 +383,6 @@
     <t>cmd:laminar/B738/knob/transponder_tara</t>
   </si>
   <si>
-    <t>cmd:laminar/B738/gpu_toggle</t>
-  </si>
-  <si>
-    <t>laminar/B738/gpu_available:1.0</t>
-  </si>
-  <si>
-    <t>set:laminar/B738/toggle_switch/capt_probes_pos=1; set:laminar/B738/toggle_switch/fo_probes_pos=1;</t>
-  </si>
-  <si>
     <t>(laminar/B738/toggle_switch/capt_probes_pos:1.0)&amp;&amp;(laminar/B738/toggle_switch/fo_probes_pos:1.0)</t>
   </si>
   <si>
@@ -485,9 +425,6 @@
     <t>cmd:laminar/B738/rotary/eng1_start_off;</t>
   </si>
   <si>
-    <t>cmdhold:0.1:laminar/B738/rotary/eng1_start_cont; cmdhold:0.1:laminar/B738/rotary/eng2_start_cont;</t>
-  </si>
-  <si>
     <t>GPU  Disconnect</t>
   </si>
   <si>
@@ -503,15 +440,6 @@
     <t>APU Online</t>
   </si>
   <si>
-    <t>FUEL_PUMP</t>
-  </si>
-  <si>
-    <t>cmd.setDataRefValue("laminar/B738/fuel/fuel_tank_pos_lft1", 1);</t>
-  </si>
-  <si>
-    <t>cmd.setDataRefValue("laminar/B738/fuel/fuel_tank_pos_lft2", 1);</t>
-  </si>
-  <si>
     <t>cmd.setDataRefValue("laminar/B738/fuel/fuel_tank_pos_ctr1", 1);</t>
   </si>
   <si>
@@ -527,18 +455,9 @@
     <t>laminar/B738/electrical/apu_bus_enable:1</t>
   </si>
   <si>
-    <t>cmdhold:1.0:laminar/B738/toggle_switch/apu_gen1_dn; cmdhold:1.0:laminar/B738/toggle_switch/apu_gen2_dn;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cmd:laminar/B738/toggle_switch/window_heat_l_fwd; cmd:laminar/B738/toggle_switch/window_heat_l_side; cmd:laminar/B738/toggle_switch/window_heat_r_fwd; cmd:laminar/B738/toggle_switch/window_heat_r_side; </t>
-  </si>
-  <si>
     <t>Window Heat ON</t>
   </si>
   <si>
-    <t>cmd:laminar/B738/fms/chock_status</t>
-  </si>
-  <si>
     <t>Chock  Wheels</t>
   </si>
   <si>
@@ -554,12 +473,6 @@
     <t>wait</t>
   </si>
   <si>
-    <t>cmdhold:2.0:laminar/B738/spring_toggle_switch/APU_start_pos_dn; cmd:laminar/B738/spring_toggle_switch/APU_start_pos_dn;</t>
-  </si>
-  <si>
-    <t>laminar/B738/fmod/gpu_deployed:1</t>
-  </si>
-  <si>
     <t>cmd:laminar/B738/rotary/eng2_start_off; cmd:laminar/B738/rotary/eng1_start_grd; cmd:laminar/B738/engine/mixture1_cutoff;</t>
   </si>
   <si>
@@ -569,7 +482,139 @@
     <t>cmd:laminar/B738/rotary/eng1_start_off; cmd:laminar/B738/rotary/eng2_start_grd; cmd:laminar/B738/engine/mixture2_cutoff;</t>
   </si>
   <si>
-    <t>Fuel Pumps On and On and On</t>
+    <t>BLOCK</t>
+  </si>
+  <si>
+    <t>GPU CONNECT</t>
+  </si>
+  <si>
+    <t>APU START</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>WHITE DOME LIGHT</t>
+  </si>
+  <si>
+    <t>GPU On</t>
+  </si>
+  <si>
+    <t>FLIGHT DECK DOOR</t>
+  </si>
+  <si>
+    <t>Open Cockpit Door</t>
+  </si>
+  <si>
+    <t>ICING WINDOW</t>
+  </si>
+  <si>
+    <t>APU GENERATOR</t>
+  </si>
+  <si>
+    <t>GPU DISCONNECT</t>
+  </si>
+  <si>
+    <t>laminar/B738/fmod/gpu_deployed:0</t>
+  </si>
+  <si>
+    <t>ICING PITOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PACKS </t>
+  </si>
+  <si>
+    <t>ENGINE_ONE CONTINUOUS</t>
+  </si>
+  <si>
+    <t>ENGINE_TWO CONTINUOUS</t>
+  </si>
+  <si>
+    <t>IRS</t>
+  </si>
+  <si>
+    <t>CLOSE_ALL_DOORS</t>
+  </si>
+  <si>
+    <t>Close All Doors</t>
+  </si>
+  <si>
+    <t>Aileron and Rudder Trim</t>
+  </si>
+  <si>
+    <t>BEACON</t>
+  </si>
+  <si>
+    <t>Beacon Lights On</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/electric_hydro_pumps1</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/electric_hydro_pumps2</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/hydro_pumps1</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/hydro_pumps2</t>
+  </si>
+  <si>
+    <t>Hydraulic Pumps On</t>
+  </si>
+  <si>
+    <t>laminar/B738/toggle_switch/electric_hydro_pumps1_pos:1</t>
+  </si>
+  <si>
+    <t>laminar/B738/toggle_switch/electric_hydro_pumps2_pos:1</t>
+  </si>
+  <si>
+    <t>laminar/B738/toggle_switch/hydro_pumps1_pos:1</t>
+  </si>
+  <si>
+    <t>laminar/B738/toggle_switch/hydro_pumps2_pos:1</t>
+  </si>
+  <si>
+    <t>FUEL PUMP</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/fuel_pump_ctr1</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/fuel_pump_ctr2</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/fuel_pump_lft1</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/fuel_pump_lft2</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/fuel_pump_rgt1</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/fuel_pump_rgt2</t>
+  </si>
+  <si>
+    <t>Fuel Pumps On</t>
+  </si>
+  <si>
+    <t>laminar/B738/fuel/fuel_tank_pos_ctr1:0</t>
+  </si>
+  <si>
+    <t>laminar/B738/fuel/fuel_tank_pos_ctr2:0</t>
+  </si>
+  <si>
+    <t>laminar/B738/fuel/fuel_tank_pos_lft1:0</t>
+  </si>
+  <si>
+    <t>laminar/B738/fuel/fuel_tank_pos_lft2:0</t>
+  </si>
+  <si>
+    <t>laminar/B738/fuel/fuel_tank_pos_rgt1:0</t>
+  </si>
+  <si>
+    <t>laminar/B738/fuel/fuel_tank_pos_rgt2:0</t>
   </si>
 </sst>
 </file>
@@ -1166,10 +1211,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}" name="ZIBO737" displayName="ZIBO737" ref="A1:L87" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L87" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L87">
-    <sortCondition ref="C1:C87"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}" name="ZIBO737" displayName="ZIBO737" ref="A1:L95" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L95" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L95">
+    <sortCondition ref="C1:C95"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{D7EB0E30-B8BB-40E3-B6DB-C78633A8AE10}" name="checklist" dataDxfId="11"/>
@@ -1506,11 +1551,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BB3736-AF94-49F8-BA64-38BE7B846CBA}">
-  <dimension ref="A1:N87"/>
+  <dimension ref="A1:N95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1559,7 +1604,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1570,7 +1615,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1587,19 +1632,19 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="I2" s="1">
         <v>1</v>
       </c>
       <c r="J2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -1621,12 +1666,12 @@
       </c>
       <c r="J3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -1648,12 +1693,12 @@
       </c>
       <c r="J4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1675,12 +1720,12 @@
       </c>
       <c r="J5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -1702,12 +1747,12 @@
       </c>
       <c r="J6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1729,12 +1774,12 @@
       </c>
       <c r="J7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -1756,12 +1801,12 @@
       </c>
       <c r="J8" s="1"/>
       <c r="L8" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1775,20 +1820,24 @@
       <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="I9" s="1">
         <v>1</v>
       </c>
       <c r="J9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -1802,25 +1851,22 @@
       <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="I10" s="1">
         <v>1</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>167</v>
-      </c>
+      <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -1834,25 +1880,22 @@
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="I11" s="1">
         <v>1</v>
       </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -1866,20 +1909,24 @@
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="I12" s="1">
         <v>1</v>
       </c>
       <c r="J12" s="1"/>
-      <c r="L12" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -1893,20 +1940,24 @@
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="I13" s="1">
         <v>1</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="L13" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -1918,42 +1969,44 @@
         <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>170</v>
-      </c>
+      <c r="H14" s="1"/>
       <c r="I14" s="1">
         <v>1</v>
       </c>
       <c r="J14" s="1"/>
-      <c r="L14" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="I15" s="1">
         <v>1</v>
       </c>
@@ -1971,19 +2024,19 @@
         <v>2</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="I16" s="1">
         <v>1</v>
@@ -2002,19 +2055,17 @@
         <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
@@ -2022,55 +2073,64 @@
       <c r="J17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" ht="57" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H18" s="1" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="I18" s="1">
         <v>1</v>
       </c>
-      <c r="J18" s="1"/>
-      <c r="L18" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
       </c>
       <c r="D19" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="I19" s="1">
         <v>1</v>
@@ -2079,105 +2139,109 @@
         <v>1</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+        <v>160</v>
+      </c>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="D20" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>151</v>
-      </c>
+      <c r="F20" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="1"/>
       <c r="I20" s="1">
         <v>1</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
       <c r="K20" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
       </c>
       <c r="D21" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1">
         <v>1</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
       <c r="K21" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1">
         <v>1</v>
       </c>
-      <c r="J22" s="1"/>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
       <c r="K22" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L22" s="1"/>
     </row>
@@ -2186,30 +2250,32 @@
         <v>11</v>
       </c>
       <c r="B23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
       </c>
       <c r="D23" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1">
         <v>1</v>
       </c>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
       <c r="K23" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L23" s="1"/>
     </row>
@@ -2218,30 +2284,32 @@
         <v>11</v>
       </c>
       <c r="B24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
       </c>
       <c r="D24" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1">
         <v>1</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
       <c r="K24" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L24" s="1"/>
     </row>
@@ -2250,123 +2318,131 @@
         <v>11</v>
       </c>
       <c r="B25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>26</v>
+        <v>157</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H25" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="I25" s="1">
         <v>1</v>
       </c>
       <c r="J25" s="1"/>
-      <c r="K25" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="57" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
       </c>
       <c r="D26" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>166</v>
-      </c>
+      <c r="F26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="1"/>
       <c r="I26" s="1">
         <v>1</v>
       </c>
-      <c r="J26" s="1"/>
-      <c r="L26" s="1" t="s">
-        <v>165</v>
-      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
       </c>
       <c r="D27" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1">
         <v>1</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
       <c r="K27" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
       </c>
       <c r="D28" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1">
         <v>1</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
       <c r="K28" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L28" s="1"/>
     </row>
@@ -2375,30 +2451,32 @@
         <v>11</v>
       </c>
       <c r="B29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
       </c>
       <c r="D29" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1">
         <v>1</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
       <c r="K29" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L29" s="1"/>
     </row>
@@ -2407,30 +2485,32 @@
         <v>11</v>
       </c>
       <c r="B30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
       </c>
       <c r="D30" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1">
         <v>1</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
       <c r="K30" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L30" s="1"/>
     </row>
@@ -2439,354 +2519,380 @@
         <v>11</v>
       </c>
       <c r="B31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
       </c>
       <c r="D31" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1">
         <v>1</v>
       </c>
-      <c r="J31" s="1"/>
+      <c r="J31" s="1">
+        <v>1</v>
+      </c>
       <c r="K31" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
       </c>
       <c r="D32" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1">
         <v>1</v>
       </c>
-      <c r="J32" s="1"/>
+      <c r="J32" s="1">
+        <v>1</v>
+      </c>
       <c r="K32" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
       </c>
       <c r="D33" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1">
         <v>1</v>
       </c>
-      <c r="J33" s="1"/>
+      <c r="J33" s="1">
+        <v>1</v>
+      </c>
       <c r="K33" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="1">
         <v>2</v>
       </c>
       <c r="D34" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1">
         <v>1</v>
       </c>
-      <c r="J34" s="1"/>
+      <c r="J34" s="1">
+        <v>1</v>
+      </c>
       <c r="K34" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="1">
         <v>2</v>
       </c>
       <c r="D35" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1">
         <v>1</v>
       </c>
-      <c r="J35" s="1"/>
+      <c r="J35" s="1">
+        <v>1</v>
+      </c>
       <c r="K35" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="1">
         <v>2</v>
       </c>
       <c r="D36" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1">
         <v>1</v>
       </c>
-      <c r="J36" s="1"/>
+      <c r="J36" s="1">
+        <v>1</v>
+      </c>
       <c r="K36" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="1">
         <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1">
         <v>1</v>
       </c>
-      <c r="J37" s="1"/>
+      <c r="J37" s="1">
+        <v>1</v>
+      </c>
       <c r="K37" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
       </c>
       <c r="D38" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1">
         <v>1</v>
       </c>
-      <c r="J38" s="1"/>
+      <c r="J38" s="1">
+        <v>1</v>
+      </c>
       <c r="K38" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
       </c>
       <c r="D39" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1">
         <v>1</v>
       </c>
-      <c r="J39" s="1"/>
+      <c r="J39" s="1">
+        <v>1</v>
+      </c>
       <c r="K39" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="1">
         <v>2</v>
       </c>
       <c r="D40" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1">
         <v>1</v>
       </c>
-      <c r="J40" s="1"/>
+      <c r="J40" s="1">
+        <v>1</v>
+      </c>
       <c r="K40" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="1">
         <v>2</v>
       </c>
       <c r="D41" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>67</v>
+        <v>180</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H41" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="I41" s="1">
         <v>1</v>
       </c>
-      <c r="J41" s="1"/>
+      <c r="J41" s="1">
+        <v>1</v>
+      </c>
       <c r="K41" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L41" s="1"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
+        <v>188</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>11</v>
       </c>
@@ -2797,30 +2903,28 @@
         <v>2</v>
       </c>
       <c r="D42" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>178</v>
-      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
       <c r="I42" s="1">
         <v>1</v>
       </c>
-      <c r="J42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="N42" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="J42" s="1">
+        <v>1</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>11</v>
       </c>
@@ -2831,31 +2935,28 @@
         <v>2</v>
       </c>
       <c r="D43" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1">
         <v>1</v>
       </c>
-      <c r="J43" s="1"/>
+      <c r="J43" s="1">
+        <v>1</v>
+      </c>
       <c r="K43" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L43" s="1"/>
-      <c r="N43" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+        <v>190</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>11</v>
       </c>
@@ -2866,31 +2967,28 @@
         <v>2</v>
       </c>
       <c r="D44" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1">
         <v>1</v>
       </c>
-      <c r="J44" s="1"/>
+      <c r="J44" s="1">
+        <v>1</v>
+      </c>
       <c r="K44" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L44" s="1"/>
-      <c r="N44" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+        <v>191</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>11</v>
       </c>
@@ -2901,31 +2999,28 @@
         <v>2</v>
       </c>
       <c r="D45" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1">
         <v>1</v>
       </c>
-      <c r="J45" s="1"/>
+      <c r="J45" s="1">
+        <v>1</v>
+      </c>
       <c r="K45" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L45" s="1"/>
-      <c r="N45" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+        <v>192</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>11</v>
       </c>
@@ -2936,31 +3031,28 @@
         <v>2</v>
       </c>
       <c r="D46" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1">
         <v>1</v>
       </c>
-      <c r="J46" s="1"/>
+      <c r="J46" s="1">
+        <v>1</v>
+      </c>
       <c r="K46" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L46" s="1"/>
-      <c r="N46" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
+        <v>193</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -2971,323 +3063,373 @@
         <v>2</v>
       </c>
       <c r="D47" s="1">
+        <v>33</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I47" s="1">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1">
+        <v>1</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1">
         <v>34</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1">
-        <v>1</v>
-      </c>
-      <c r="J47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="N47" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="L48" s="1"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A49" s="1"/>
+      <c r="I48" s="1">
+        <v>1</v>
+      </c>
+      <c r="J48" s="1">
+        <v>1</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B49" s="1">
         <v>1</v>
       </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
+      <c r="C49" s="1">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>35</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="L49" s="1"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I49" s="1">
+        <v>1</v>
+      </c>
+      <c r="J49" s="1">
+        <v>1</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
       </c>
       <c r="C50" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D50" s="1">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
       <c r="I50" s="1">
         <v>1</v>
       </c>
-      <c r="J50" s="1"/>
+      <c r="J50" s="1">
+        <v>1</v>
+      </c>
       <c r="K50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L50" s="1"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+        <v>179</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="B51" s="1">
         <v>1</v>
       </c>
       <c r="C51" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D51" s="1">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
+        <v>169</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="I51" s="1">
         <v>1</v>
       </c>
-      <c r="J51" s="1"/>
+      <c r="J51" s="1">
+        <v>1</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="L51" s="1"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A52" s="1"/>
+      <c r="N51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A52" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B52" s="1">
         <v>1</v>
       </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="C52" s="1">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>38</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
+      <c r="H52" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I52" s="1">
+        <v>1</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="L52" s="1"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A53" s="1"/>
+      <c r="N52" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A53" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B53" s="1">
         <v>1</v>
       </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="C53" s="1">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1">
+        <v>39</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
+      <c r="H53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I53" s="1">
+        <v>1</v>
+      </c>
+      <c r="J53" s="1">
+        <v>1</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="L53" s="1"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="N53" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="B54" s="1">
         <v>1</v>
       </c>
       <c r="C54" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D54" s="1">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1">
         <v>1</v>
       </c>
       <c r="J54" s="1"/>
       <c r="L54" s="1"/>
-    </row>
-    <row r="55" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A55" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="N54" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A55" s="1"/>
       <c r="B55" s="1">
         <v>1</v>
       </c>
-      <c r="C55" s="1">
-        <v>4</v>
-      </c>
-      <c r="D55" s="1">
-        <v>2</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I55" s="1">
-        <v>1</v>
-      </c>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
       <c r="J55" s="1"/>
-      <c r="L55" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A56" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="L55" s="1"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A56" s="1"/>
       <c r="B56" s="1">
         <v>1</v>
       </c>
-      <c r="C56" s="1">
-        <v>4</v>
-      </c>
-      <c r="D56" s="1">
-        <v>3</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="I56" s="1">
-        <v>1</v>
-      </c>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
       </c>
       <c r="C57" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D57" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="F57" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="H57" s="1" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="I57" s="1">
         <v>1</v>
       </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+      <c r="L57" s="1"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B58" s="1">
         <v>1</v>
       </c>
       <c r="C58" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D58" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="G58" s="1"/>
-      <c r="H58" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="H58" s="1"/>
       <c r="I58" s="1">
         <v>1</v>
       </c>
       <c r="J58" s="1"/>
-      <c r="K58" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A59" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="L58" s="1"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A59" s="1"/>
       <c r="B59" s="1">
         <v>1</v>
       </c>
-      <c r="C59" s="1">
-        <v>4</v>
-      </c>
-      <c r="D59" s="1">
-        <v>6</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-      <c r="I59" s="1">
-        <v>1</v>
-      </c>
+      <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
       <c r="B60" s="1">
         <v>1</v>
@@ -3302,62 +3444,76 @@
       <c r="J60" s="1"/>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A61" s="1"/>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="B61" s="1">
         <v>1</v>
       </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
+      <c r="C61" s="1">
+        <v>4</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
+      <c r="I61" s="1">
+        <v>1</v>
+      </c>
       <c r="J61" s="1"/>
       <c r="L61" s="1"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B62" s="1">
         <v>1</v>
       </c>
       <c r="C62" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D62" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="I62" s="1">
         <v>1</v>
       </c>
       <c r="J62" s="1"/>
-      <c r="L62" s="1"/>
-    </row>
-    <row r="63" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="L62" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B63" s="1">
         <v>1</v>
       </c>
       <c r="C63" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D63" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>12</v>
@@ -3365,28 +3521,26 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="I63" s="1">
         <v>1</v>
       </c>
       <c r="J63" s="1"/>
-      <c r="L63" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L63" s="1"/>
+    </row>
+    <row r="64" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
       </c>
       <c r="C64" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D64" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>12</v>
@@ -3394,26 +3548,33 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="I64" s="1">
         <v>1</v>
       </c>
-      <c r="J64" s="1"/>
-      <c r="L64" s="1"/>
+      <c r="J64" s="1">
+        <v>1</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="65" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B65" s="1">
         <v>1</v>
       </c>
       <c r="C65" s="1">
+        <v>4</v>
+      </c>
+      <c r="D65" s="1">
         <v>5</v>
-      </c>
-      <c r="D65" s="1">
-        <v>4</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>12</v>
@@ -3421,75 +3582,60 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="I65" s="1">
         <v>1</v>
       </c>
-      <c r="J65" s="1"/>
+      <c r="J65" s="1">
+        <v>1</v>
+      </c>
       <c r="K65" s="1" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B66" s="1">
         <v>1</v>
       </c>
       <c r="C66" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D66" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G66" s="1"/>
-      <c r="H66" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="H66" s="1"/>
       <c r="I66" s="1">
         <v>1</v>
       </c>
       <c r="J66" s="1"/>
-      <c r="K66" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>148</v>
-      </c>
+      <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A67" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="A67" s="1"/>
       <c r="B67" s="1">
         <v>1</v>
       </c>
-      <c r="C67" s="1">
-        <v>5</v>
-      </c>
-      <c r="D67" s="1">
-        <v>6</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
-      <c r="I67" s="1">
-        <v>1</v>
-      </c>
+      <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="L67" s="1"/>
     </row>
@@ -3509,249 +3655,218 @@
       <c r="L68" s="1"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A69" s="1"/>
+      <c r="A69" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="B69" s="1">
         <v>1</v>
       </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
+      <c r="C69" s="1">
+        <v>5</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
+      <c r="I69" s="1">
+        <v>1</v>
+      </c>
       <c r="J69" s="1"/>
       <c r="L69" s="1"/>
     </row>
     <row r="70" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B70" s="1">
         <v>1</v>
       </c>
       <c r="C70" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D70" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="I70" s="1">
         <v>1</v>
       </c>
       <c r="J70" s="1"/>
-      <c r="K70" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L70" s="1"/>
-    </row>
-    <row r="71" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="L70" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B71" s="1">
         <v>1</v>
       </c>
       <c r="C71" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D71" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="I71" s="1">
         <v>1</v>
       </c>
       <c r="J71" s="1"/>
-      <c r="K71" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="L71" s="1" t="s">
-        <v>135</v>
-      </c>
+      <c r="L71" s="1"/>
     </row>
     <row r="72" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B72" s="1">
         <v>1</v>
       </c>
       <c r="C72" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D72" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="I72" s="1">
         <v>1</v>
       </c>
-      <c r="J72" s="1"/>
+      <c r="J72" s="1">
+        <v>1</v>
+      </c>
       <c r="K72" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L72" s="1"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B73" s="1">
         <v>1</v>
       </c>
       <c r="C73" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D73" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="I73" s="1">
         <v>1</v>
       </c>
-      <c r="J73" s="1"/>
+      <c r="J73" s="1">
+        <v>1</v>
+      </c>
       <c r="K73" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L73" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B74" s="1">
         <v>1</v>
       </c>
       <c r="C74" s="1">
+        <v>5</v>
+      </c>
+      <c r="D74" s="1">
         <v>6</v>
       </c>
-      <c r="D74" s="1">
-        <v>5</v>
-      </c>
       <c r="E74" s="1" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="G74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1">
         <v>1</v>
       </c>
       <c r="J74" s="1"/>
-      <c r="K74" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="L74" s="1"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A75" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="A75" s="1"/>
       <c r="B75" s="1">
         <v>1</v>
       </c>
-      <c r="C75" s="1">
-        <v>6</v>
-      </c>
-      <c r="D75" s="1">
-        <v>6</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
       <c r="H75" s="1"/>
-      <c r="I75" s="1">
-        <v>1</v>
-      </c>
+      <c r="I75" s="1"/>
       <c r="J75" s="1"/>
-      <c r="K75" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="L75" s="1"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A76" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="A76" s="1"/>
       <c r="B76" s="1">
         <v>1</v>
       </c>
-      <c r="C76" s="1">
-        <v>6</v>
-      </c>
-      <c r="D76" s="1">
-        <v>7</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
       <c r="H76" s="1"/>
-      <c r="I76" s="1">
-        <v>1</v>
-      </c>
+      <c r="I76" s="1"/>
       <c r="J76" s="1"/>
-      <c r="K76" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="L76" s="1"/>
     </row>
-    <row r="77" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B77" s="1">
         <v>1</v>
@@ -3760,29 +3875,27 @@
         <v>6</v>
       </c>
       <c r="D77" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>114</v>
+        <v>14</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1">
         <v>1</v>
       </c>
       <c r="J77" s="1"/>
-      <c r="L77" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L77" s="1"/>
+    </row>
+    <row r="78" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B78" s="1">
         <v>1</v>
@@ -3791,29 +3904,32 @@
         <v>6</v>
       </c>
       <c r="D78" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G78" s="1">
-        <v>5</v>
+        <v>161</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1">
         <v>1</v>
       </c>
-      <c r="J78" s="1"/>
-      <c r="L78" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="J78" s="1">
+        <v>1</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L78" s="1"/>
     </row>
     <row r="79" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B79" s="1">
         <v>1</v>
@@ -3822,30 +3938,32 @@
         <v>6</v>
       </c>
       <c r="D79" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1">
         <v>1</v>
       </c>
-      <c r="J79" s="1"/>
+      <c r="J79" s="1">
+        <v>1</v>
+      </c>
       <c r="K79" s="1" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="L79" s="1"/>
     </row>
-    <row r="80" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B80" s="1">
         <v>1</v>
@@ -3854,29 +3972,32 @@
         <v>6</v>
       </c>
       <c r="D80" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1">
         <v>1</v>
       </c>
-      <c r="J80" s="1"/>
-      <c r="L80" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="J80" s="1">
+        <v>1</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L80" s="1"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B81" s="1">
         <v>1</v>
@@ -3885,202 +4006,450 @@
         <v>6</v>
       </c>
       <c r="D81" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G81" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1">
         <v>1</v>
       </c>
-      <c r="J81" s="1"/>
+      <c r="J81" s="1">
+        <v>1</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="L81" s="1"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="B82" s="1">
         <v>1</v>
       </c>
       <c r="C82" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D82" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
+      <c r="F82" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1">
         <v>1</v>
       </c>
-      <c r="J82" s="1"/>
+      <c r="J82" s="1">
+        <v>1</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="L82" s="1"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="B83" s="1">
         <v>1</v>
       </c>
       <c r="C83" s="1">
+        <v>6</v>
+      </c>
+      <c r="D83" s="1">
         <v>7</v>
       </c>
-      <c r="D83" s="1">
-        <v>2</v>
-      </c>
       <c r="E83" s="1" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G83" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1">
         <v>1</v>
       </c>
-      <c r="J83" s="1"/>
+      <c r="J83" s="1">
+        <v>1</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="L83" s="1"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="B84" s="1">
         <v>1</v>
       </c>
       <c r="C84" s="1">
+        <v>6</v>
+      </c>
+      <c r="D84" s="1">
         <v>8</v>
       </c>
-      <c r="D84" s="1">
-        <v>1</v>
-      </c>
       <c r="E84" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="G84" s="1"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1">
         <v>1</v>
       </c>
       <c r="J84" s="1"/>
-      <c r="K84" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="L84" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="L84" s="1"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="B85" s="1">
         <v>1</v>
       </c>
       <c r="C85" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D85" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1">
         <v>1</v>
       </c>
       <c r="J85" s="1"/>
-      <c r="L85" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="L85" s="1"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="B86" s="1">
         <v>1</v>
       </c>
       <c r="C86" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D86" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>128</v>
+        <v>101</v>
+      </c>
+      <c r="G86" s="1">
+        <v>5</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1">
         <v>1</v>
       </c>
       <c r="J86" s="1"/>
-      <c r="L86" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L86" s="1"/>
+    </row>
+    <row r="87" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="B87" s="1">
         <v>1</v>
       </c>
       <c r="C87" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D87" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>129</v>
+        <v>14</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1">
         <v>1</v>
       </c>
-      <c r="J87" s="1"/>
+      <c r="J87" s="1">
+        <v>1</v>
+      </c>
       <c r="K87" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="L87" s="1" t="s">
-        <v>132</v>
+        <v>103</v>
+      </c>
+      <c r="L87" s="1"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A88" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" s="1">
+        <v>1</v>
+      </c>
+      <c r="C88" s="1">
+        <v>6</v>
+      </c>
+      <c r="D88" s="1">
+        <v>12</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1">
+        <v>1</v>
+      </c>
+      <c r="J88" s="1"/>
+      <c r="L88" s="1"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A89" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" s="1">
+        <v>1</v>
+      </c>
+      <c r="C89" s="1">
+        <v>6</v>
+      </c>
+      <c r="D89" s="1">
+        <v>13</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1">
+        <v>1</v>
+      </c>
+      <c r="J89" s="1"/>
+      <c r="L89" s="1"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A90" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B90" s="1">
+        <v>1</v>
+      </c>
+      <c r="C90" s="1">
+        <v>7</v>
+      </c>
+      <c r="D90" s="1">
+        <v>1</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1">
+        <v>1</v>
+      </c>
+      <c r="J90" s="1"/>
+      <c r="L90" s="1"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A91" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B91" s="1">
+        <v>1</v>
+      </c>
+      <c r="C91" s="1">
+        <v>7</v>
+      </c>
+      <c r="D91" s="1">
+        <v>2</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1">
+        <v>1</v>
+      </c>
+      <c r="J91" s="1"/>
+      <c r="L91" s="1"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A92" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B92" s="1">
+        <v>1</v>
+      </c>
+      <c r="C92" s="1">
+        <v>8</v>
+      </c>
+      <c r="D92" s="1">
+        <v>1</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1">
+        <v>1</v>
+      </c>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L92" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A93" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93" s="1">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1">
+        <v>8</v>
+      </c>
+      <c r="D93" s="1">
+        <v>2</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1">
+        <v>1</v>
+      </c>
+      <c r="J93" s="1"/>
+      <c r="L93" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A94" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B94" s="1">
+        <v>1</v>
+      </c>
+      <c r="C94" s="1">
+        <v>8</v>
+      </c>
+      <c r="D94" s="1">
+        <v>3</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1">
+        <v>1</v>
+      </c>
+      <c r="J94" s="1"/>
+      <c r="L94" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A95" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B95" s="1">
+        <v>1</v>
+      </c>
+      <c r="C95" s="1">
+        <v>8</v>
+      </c>
+      <c r="D95" s="1">
+        <v>4</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1">
+        <v>1</v>
+      </c>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L95" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Control page and update checklists spreadsheet
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/CopilotAI_Checklists.xlsx
+++ b/CopilotAI_Checklists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnl\Documents\projects\CopilotAI\claude_shell_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CE2CFD-2AD0-42F2-9103-83887D023FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069DAABC-7B0F-4B39-94AC-2734E9A61BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57840" yWindow="-98" windowWidth="28995" windowHeight="16395" xr2:uid="{B7C423D5-FDD5-4D99-96F7-653924CCE03F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="165">
   <si>
     <t>checklist</t>
   </si>
@@ -80,9 +80,6 @@
     <t>ON</t>
   </si>
   <si>
-    <t>NAV</t>
-  </si>
-  <si>
     <t>laminar/B738/toggle_switch/no_smoking_pos:&gt;0.0</t>
   </si>
   <si>
@@ -254,12 +251,6 @@
     <t>Brake On</t>
   </si>
   <si>
-    <t>Start APU</t>
-  </si>
-  <si>
-    <t>APU Online</t>
-  </si>
-  <si>
     <t>cmd.setDataRefValue("laminar/B738/fuel/fuel_tank_pos_ctr1", 1);</t>
   </si>
   <si>
@@ -320,12 +311,6 @@
     <t>ICING WINDOW</t>
   </si>
   <si>
-    <t>APU GENERATOR</t>
-  </si>
-  <si>
-    <t>GPU DISCONNECT</t>
-  </si>
-  <si>
     <t>laminar/B738/fmod/gpu_deployed:0</t>
   </si>
   <si>
@@ -341,9 +326,6 @@
     <t>ENGINE_TWO CONTINUOUS</t>
   </si>
   <si>
-    <t>IRS</t>
-  </si>
-  <si>
     <t>CLOSE_ALL_DOORS</t>
   </si>
   <si>
@@ -386,9 +368,6 @@
     <t>Fuel Pumps On</t>
   </si>
   <si>
-    <t>IRS switch to NAV</t>
-  </si>
-  <si>
     <t>FUEL_PUMP</t>
   </si>
   <si>
@@ -522,6 +501,33 @@
   </si>
   <si>
     <t>laminar/B738/air/isolation_valve_pos:1</t>
+  </si>
+  <si>
+    <t>IRS_NAV</t>
+  </si>
+  <si>
+    <t>Command IRS switchs to align</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/irs_L_right; cmd:laminar/B738/toggle_switch/irs_R_right; cmd:sleep(2000);</t>
+  </si>
+  <si>
+    <t>Initialize FMS Position and Flight Plan</t>
+  </si>
+  <si>
+    <t>Start APU and Wait till APU Power is Available</t>
+  </si>
+  <si>
+    <t>cmd.sendCommand("laminar/B738/toggle_switch/apu_gen1_dn");</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/apu_gen1_dn; cmd sleep (500); cmd:laminar/B738/toggle_switch/apu_gen2_dn;</t>
+  </si>
+  <si>
+    <t>Place both APU Generators online.</t>
+  </si>
+  <si>
+    <t>cmd: laminar/B738/gpu_toggle</t>
   </si>
 </sst>
 </file>
@@ -1118,10 +1124,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}" name="ZIBO737" displayName="ZIBO737" ref="A1:L86" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L86" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L86">
-    <sortCondition ref="C1:C86"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}" name="ZIBO737" displayName="ZIBO737" ref="A1:L87" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L87" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L87">
+    <sortCondition ref="C1:C87"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{D7EB0E30-B8BB-40E3-B6DB-C78633A8AE10}" name="checklist" dataDxfId="11"/>
@@ -1458,11 +1464,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BB3736-AF94-49F8-BA64-38BE7B846CBA}">
-  <dimension ref="A1:N86"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1482,7 +1488,7 @@
     <col min="13" max="13" width="21.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1511,7 +1517,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1520,9 +1526,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1539,7 +1545,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I2" s="1">
         <v>1</v>
@@ -1547,9 +1553,9 @@
       <c r="J2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -1564,7 +1570,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1574,9 +1580,9 @@
       <c r="J3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -1591,7 +1597,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1601,9 +1607,9 @@
       <c r="J4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1618,7 +1624,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1628,9 +1634,9 @@
       <c r="J5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -1645,11 +1651,11 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
@@ -1657,9 +1663,9 @@
       <c r="J6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1671,45 +1677,41 @@
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="H7" s="1"/>
       <c r="I7" s="1">
         <v>1</v>
       </c>
       <c r="J7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>
@@ -1717,30 +1719,30 @@
       <c r="J8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="I9" s="1">
         <v>1</v>
@@ -1748,34 +1750,38 @@
       <c r="J9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="I10" s="1">
         <v>1</v>
       </c>
       <c r="J10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1786,19 +1792,19 @@
         <v>2</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="I11" s="1">
         <v>1</v>
@@ -1806,7 +1812,7 @@
       <c r="J11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1817,19 +1823,19 @@
         <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I12" s="1">
         <v>1</v>
@@ -1837,7 +1843,7 @@
       <c r="J12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1848,25 +1854,25 @@
         <v>2</v>
       </c>
       <c r="D13" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>73</v>
+        <v>157</v>
       </c>
       <c r="I13" s="1">
         <v>1</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L13" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1877,32 +1883,25 @@
         <v>2</v>
       </c>
       <c r="D14" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="I14" s="1">
         <v>1</v>
       </c>
-      <c r="J14" s="1">
-        <v>1</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="J14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1913,17 +1912,13 @@
         <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>5</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>70</v>
+        <v>163</v>
       </c>
       <c r="I15" s="1">
         <v>1</v>
@@ -1932,11 +1927,16 @@
         <v>1</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="N15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1947,27 +1947,30 @@
         <v>2</v>
       </c>
       <c r="D16" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="I16" s="1">
         <v>1</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1978,16 +1981,18 @@
         <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="I17" s="1">
         <v>1</v>
       </c>
@@ -2005,25 +2010,20 @@
         <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="H18" s="1"/>
       <c r="I18" s="1">
         <v>1</v>
       </c>
-      <c r="J18" s="1">
-        <v>1</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="J18" s="1"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
@@ -2037,22 +2037,25 @@
         <v>2</v>
       </c>
       <c r="D19" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="I19" s="1">
         <v>1</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
@@ -2066,16 +2069,16 @@
         <v>2</v>
       </c>
       <c r="D20" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1">
@@ -2095,20 +2098,18 @@
         <v>2</v>
       </c>
       <c r="D21" s="1">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="H21" s="1"/>
       <c r="I21" s="1">
         <v>1</v>
       </c>
@@ -2126,25 +2127,24 @@
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H22" s="1" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="I22" s="1">
         <v>1</v>
       </c>
-      <c r="J22" s="1">
-        <v>1</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="J22" s="1"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
@@ -2158,7 +2158,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>12</v>
@@ -2166,7 +2166,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I23" s="1">
         <v>1</v>
@@ -2175,13 +2175,11 @@
         <v>1</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -2192,7 +2190,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="1">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
@@ -2200,7 +2198,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I24" s="1">
         <v>1</v>
@@ -2209,9 +2207,11 @@
         <v>1</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L24" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
@@ -2224,7 +2224,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>12</v>
@@ -2232,7 +2232,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="I25" s="1">
         <v>1</v>
@@ -2241,7 +2241,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L25" s="1"/>
     </row>
@@ -2256,7 +2256,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="1">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>12</v>
@@ -2264,7 +2264,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
@@ -2273,7 +2273,7 @@
         <v>1</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L26" s="1"/>
     </row>
@@ -2288,50 +2288,50 @@
         <v>2</v>
       </c>
       <c r="D27" s="1">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
         <v>21</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1">
-        <v>1</v>
-      </c>
-      <c r="J27" s="1">
-        <v>1</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1">
-        <v>2</v>
-      </c>
-      <c r="D28" s="1">
-        <v>18</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="H28" s="1"/>
       <c r="I28" s="1">
         <v>1</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L28" s="1"/>
     </row>
@@ -2354,7 +2354,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
@@ -2362,7 +2362,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="I29" s="1">
         <v>1</v>
@@ -2371,7 +2371,7 @@
         <v>1</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L29" s="1"/>
     </row>
@@ -2386,7 +2386,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="1">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>12</v>
@@ -2394,7 +2394,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="I30" s="1">
         <v>1</v>
@@ -2403,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L30" s="1"/>
     </row>
@@ -2418,27 +2418,28 @@
         <v>2</v>
       </c>
       <c r="D31" s="1">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
         <v>128</v>
       </c>
       <c r="I31" s="1">
         <v>1</v>
       </c>
-      <c r="J31" s="1"/>
+      <c r="J31" s="1">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
@@ -2449,19 +2450,19 @@
         <v>2</v>
       </c>
       <c r="D32" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>142</v>
+        <v>26</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="I32" s="1">
         <v>1</v>
@@ -2469,7 +2470,7 @@
       <c r="J32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
@@ -2480,25 +2481,24 @@
         <v>2</v>
       </c>
       <c r="D33" s="1">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="H33" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I33" s="1">
         <v>1</v>
       </c>
-      <c r="J33" s="1">
-        <v>1</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="J33" s="1"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.45">
@@ -2512,7 +2512,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="1">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>12</v>
@@ -2520,7 +2520,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="I34" s="1">
         <v>1</v>
@@ -2529,73 +2529,73 @@
         <v>1</v>
       </c>
       <c r="K34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>28</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1</v>
+      </c>
+      <c r="J35" s="1">
+        <v>1</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>29</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L34" s="1"/>
-    </row>
-    <row r="35" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="1">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1">
-        <v>2</v>
-      </c>
-      <c r="D35" s="1">
-        <v>25</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H36" s="1"/>
+      <c r="I36" s="1">
+        <v>1</v>
+      </c>
+      <c r="J36" s="1">
+        <v>1</v>
+      </c>
+      <c r="K36" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1">
-        <v>1</v>
-      </c>
-      <c r="J35" s="1">
-        <v>1</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L35" s="1"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="1">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1">
-        <v>2</v>
-      </c>
-      <c r="D36" s="1">
-        <v>26</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I36" s="1">
-        <v>1</v>
-      </c>
-      <c r="J36" s="1">
-        <v>1</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="L36" s="1"/>
     </row>
@@ -2610,24 +2610,25 @@
         <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="I37" s="1">
         <v>1</v>
       </c>
-      <c r="J37" s="1"/>
+      <c r="J37" s="1">
+        <v>1</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.45">
@@ -2641,28 +2642,25 @@
         <v>2</v>
       </c>
       <c r="D38" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H38" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I38" s="1">
         <v>1</v>
       </c>
-      <c r="J38" s="1">
-        <v>1</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="J38" s="1"/>
+      <c r="L38" s="1"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
@@ -2675,14 +2673,16 @@
         <v>2</v>
       </c>
       <c r="D39" s="1">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="I39" s="1">
         <v>1</v>
       </c>
@@ -2690,10 +2690,10 @@
         <v>1</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.45">
@@ -2707,7 +2707,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>12</v>
@@ -2722,10 +2722,10 @@
         <v>1</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.45">
@@ -2739,7 +2739,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="1">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>12</v>
@@ -2754,10 +2754,10 @@
         <v>1</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.45">
@@ -2771,28 +2771,28 @@
         <v>2</v>
       </c>
       <c r="D42" s="1">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1">
         <v>1</v>
       </c>
-      <c r="J42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="N42" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="J42" s="1">
+        <v>1</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>11</v>
       </c>
@@ -2803,31 +2803,28 @@
         <v>2</v>
       </c>
       <c r="D43" s="1">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="F43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" s="1"/>
       <c r="I43" s="1">
         <v>1</v>
       </c>
-      <c r="J43" s="1">
-        <v>1</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="J43" s="1"/>
       <c r="L43" s="1"/>
       <c r="N43" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>11</v>
       </c>
@@ -2838,25 +2835,28 @@
         <v>2</v>
       </c>
       <c r="D44" s="1">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>103</v>
-      </c>
+      <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I44" s="1">
         <v>1</v>
       </c>
-      <c r="J44" s="1"/>
+      <c r="J44" s="1">
+        <v>1</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="L44" s="1"/>
       <c r="N44" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.45">
@@ -2870,39 +2870,56 @@
         <v>2</v>
       </c>
       <c r="D45" s="1">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
+      <c r="H45" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="I45" s="1">
         <v>1</v>
       </c>
       <c r="J45" s="1"/>
       <c r="L45" s="1"/>
       <c r="N45" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B46" s="1">
         <v>1</v>
       </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>39</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
+      <c r="I46" s="1">
+        <v>1</v>
+      </c>
       <c r="J46" s="1"/>
       <c r="L46" s="1"/>
+      <c r="N46" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A47" s="1"/>
@@ -2920,37 +2937,23 @@
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A48" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A48" s="1"/>
       <c r="B48" s="1">
         <v>1</v>
       </c>
-      <c r="C48" s="1">
-        <v>3</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I48" s="1">
-        <v>1</v>
-      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="L48" s="1"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
@@ -2959,16 +2962,18 @@
         <v>3</v>
       </c>
       <c r="D49" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+      <c r="H49" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="I49" s="1">
         <v>1</v>
       </c>
@@ -2976,17 +2981,29 @@
       <c r="L49" s="1"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="B50" s="1">
         <v>1</v>
       </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="C50" s="1">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
+      <c r="I50" s="1">
+        <v>1</v>
+      </c>
       <c r="J50" s="1"/>
       <c r="L50" s="1"/>
     </row>
@@ -3006,37 +3023,23 @@
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A52" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="A52" s="1"/>
       <c r="B52" s="1">
         <v>1</v>
       </c>
-      <c r="C52" s="1">
-        <v>4</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
       <c r="H52" s="1"/>
-      <c r="I52" s="1">
-        <v>1</v>
-      </c>
+      <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B53" s="1">
         <v>1</v>
@@ -3045,27 +3048,27 @@
         <v>4</v>
       </c>
       <c r="D53" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="F53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" s="1"/>
       <c r="I53" s="1">
         <v>1</v>
       </c>
       <c r="J53" s="1"/>
-      <c r="L53" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L53" s="1"/>
+    </row>
+    <row r="54" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B54" s="1">
         <v>1</v>
@@ -3074,7 +3077,7 @@
         <v>4</v>
       </c>
       <c r="D54" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>12</v>
@@ -3082,17 +3085,19 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I54" s="1">
         <v>1</v>
       </c>
       <c r="J54" s="1"/>
-      <c r="L54" s="1"/>
-    </row>
-    <row r="55" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="L54" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B55" s="1">
         <v>1</v>
@@ -3101,7 +3106,7 @@
         <v>4</v>
       </c>
       <c r="D55" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>12</v>
@@ -3109,24 +3114,17 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I55" s="1">
         <v>1</v>
       </c>
-      <c r="J55" s="1">
-        <v>1</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="J55" s="1"/>
+      <c r="L55" s="1"/>
     </row>
     <row r="56" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B56" s="1">
         <v>1</v>
@@ -3135,7 +3133,7 @@
         <v>4</v>
       </c>
       <c r="D56" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>12</v>
@@ -3143,7 +3141,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I56" s="1">
         <v>1</v>
@@ -3152,15 +3150,15 @@
         <v>1</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
@@ -3169,34 +3167,53 @@
         <v>4</v>
       </c>
       <c r="D57" s="1">
+        <v>5</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I57" s="1">
+        <v>1</v>
+      </c>
+      <c r="J57" s="1">
+        <v>1</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A58" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1">
+        <v>4</v>
+      </c>
+      <c r="D58" s="1">
         <v>6</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1">
-        <v>1</v>
-      </c>
-      <c r="J57" s="1"/>
-      <c r="L57" s="1"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1">
-        <v>1</v>
-      </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
+      <c r="I58" s="1">
+        <v>1</v>
+      </c>
       <c r="J58" s="1"/>
       <c r="L58" s="1"/>
     </row>
@@ -3216,37 +3233,23 @@
       <c r="L59" s="1"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A60" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A60" s="1"/>
       <c r="B60" s="1">
         <v>1</v>
       </c>
-      <c r="C60" s="1">
-        <v>5</v>
-      </c>
-      <c r="D60" s="1">
-        <v>1</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
       <c r="H60" s="1"/>
-      <c r="I60" s="1">
-        <v>1</v>
-      </c>
+      <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B61" s="1">
         <v>1</v>
@@ -3255,27 +3258,27 @@
         <v>5</v>
       </c>
       <c r="D61" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="F61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61" s="1"/>
       <c r="I61" s="1">
         <v>1</v>
       </c>
       <c r="J61" s="1"/>
-      <c r="L61" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L61" s="1"/>
+    </row>
+    <row r="62" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B62" s="1">
         <v>1</v>
@@ -3284,7 +3287,7 @@
         <v>5</v>
       </c>
       <c r="D62" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>12</v>
@@ -3298,11 +3301,13 @@
         <v>1</v>
       </c>
       <c r="J62" s="1"/>
-      <c r="L62" s="1"/>
-    </row>
-    <row r="63" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="L62" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B63" s="1">
         <v>1</v>
@@ -3311,7 +3316,7 @@
         <v>5</v>
       </c>
       <c r="D63" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>12</v>
@@ -3319,24 +3324,17 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I63" s="1">
         <v>1</v>
       </c>
-      <c r="J63" s="1">
-        <v>1</v>
-      </c>
-      <c r="K63" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="J63" s="1"/>
+      <c r="L63" s="1"/>
     </row>
     <row r="64" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
@@ -3345,7 +3343,7 @@
         <v>5</v>
       </c>
       <c r="D64" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>12</v>
@@ -3353,7 +3351,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I64" s="1">
         <v>1</v>
@@ -3362,15 +3360,15 @@
         <v>1</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B65" s="1">
         <v>1</v>
@@ -3379,34 +3377,53 @@
         <v>5</v>
       </c>
       <c r="D65" s="1">
+        <v>5</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I65" s="1">
+        <v>1</v>
+      </c>
+      <c r="J65" s="1">
+        <v>1</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A66" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1</v>
+      </c>
+      <c r="C66" s="1">
+        <v>5</v>
+      </c>
+      <c r="D66" s="1">
         <v>6</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1">
-        <v>1</v>
-      </c>
-      <c r="J65" s="1"/>
-      <c r="L65" s="1"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1">
-        <v>1</v>
-      </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
+      <c r="E66" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
+      <c r="I66" s="1">
+        <v>1</v>
+      </c>
       <c r="J66" s="1"/>
       <c r="L66" s="1"/>
     </row>
@@ -3426,39 +3443,23 @@
       <c r="L67" s="1"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A68" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="A68" s="1"/>
       <c r="B68" s="1">
         <v>1</v>
       </c>
-      <c r="C68" s="1">
-        <v>6</v>
-      </c>
-      <c r="D68" s="1">
-        <v>1</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I68" s="1">
-        <v>1</v>
-      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="L68" s="1"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B69" s="1">
         <v>1</v>
@@ -3467,19 +3468,19 @@
         <v>6</v>
       </c>
       <c r="D69" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="I69" s="1">
         <v>1</v>
@@ -3489,7 +3490,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B70" s="1">
         <v>1</v>
@@ -3498,18 +3499,20 @@
         <v>6</v>
       </c>
       <c r="D70" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H70" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="I70" s="1">
         <v>1</v>
       </c>
@@ -3518,7 +3521,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B71" s="1">
         <v>1</v>
@@ -3527,30 +3530,27 @@
         <v>6</v>
       </c>
       <c r="D71" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1" t="s">
-        <v>157</v>
-      </c>
+      <c r="F71" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H71" s="1"/>
       <c r="I71" s="1">
         <v>1</v>
       </c>
       <c r="J71" s="1"/>
-      <c r="K71" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L71" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="L71" s="1"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B72" s="1">
         <v>1</v>
@@ -3559,30 +3559,30 @@
         <v>6</v>
       </c>
       <c r="D72" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="I72" s="1">
         <v>1</v>
       </c>
       <c r="J72" s="1"/>
       <c r="K72" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L72" s="1"/>
+        <v>155</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" s="1">
         <v>1</v>
@@ -3591,29 +3591,30 @@
         <v>6</v>
       </c>
       <c r="D73" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>149</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H73" s="1"/>
       <c r="I73" s="1">
         <v>1</v>
       </c>
       <c r="J73" s="1"/>
+      <c r="K73" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="L73" s="1"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B74" s="1">
         <v>1</v>
@@ -3622,19 +3623,19 @@
         <v>6</v>
       </c>
       <c r="D74" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I74" s="1">
         <v>1</v>
@@ -3644,7 +3645,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B75" s="1">
         <v>1</v>
@@ -3653,17 +3654,19 @@
         <v>6</v>
       </c>
       <c r="D75" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G75" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="H75" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="I75" s="1">
         <v>1</v>
@@ -3673,7 +3676,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B76" s="1">
         <v>1</v>
@@ -3682,17 +3685,17 @@
         <v>6</v>
       </c>
       <c r="D76" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G76" s="1"/>
       <c r="H76" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I76" s="1">
         <v>1</v>
@@ -3702,7 +3705,7 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B77" s="1">
         <v>1</v>
@@ -3711,19 +3714,17 @@
         <v>6</v>
       </c>
       <c r="D77" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G77" s="1">
-        <v>5</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="G77" s="1"/>
       <c r="H77" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="I77" s="1">
         <v>1</v>
@@ -3733,7 +3734,7 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B78" s="1">
         <v>1</v>
@@ -3742,19 +3743,19 @@
         <v>6</v>
       </c>
       <c r="D78" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
+      </c>
+      <c r="G78" s="1">
+        <v>5</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="I78" s="1">
         <v>1</v>
@@ -3764,7 +3765,7 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B79" s="1">
         <v>1</v>
@@ -3773,19 +3774,19 @@
         <v>6</v>
       </c>
       <c r="D79" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="I79" s="1">
         <v>1</v>
@@ -3795,7 +3796,7 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B80" s="1">
         <v>1</v>
@@ -3804,16 +3805,20 @@
         <v>6</v>
       </c>
       <c r="D80" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="I80" s="1">
         <v>1</v>
       </c>
@@ -3822,21 +3827,23 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B81" s="1">
         <v>1</v>
       </c>
       <c r="C81" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D81" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F81" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1">
@@ -3847,7 +3854,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B82" s="1">
         <v>1</v>
@@ -3856,14 +3863,12 @@
         <v>7</v>
       </c>
       <c r="D82" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1">
@@ -3874,29 +3879,25 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B83" s="1">
         <v>1</v>
       </c>
       <c r="C83" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D83" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>156</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
       <c r="I83" s="1">
         <v>1</v>
       </c>
@@ -3905,7 +3906,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B84" s="1">
         <v>1</v>
@@ -3914,19 +3915,19 @@
         <v>8</v>
       </c>
       <c r="D84" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>159</v>
+        <v>50</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I84" s="1">
         <v>1</v>
@@ -3936,7 +3937,7 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B85" s="1">
         <v>1</v>
@@ -3945,19 +3946,19 @@
         <v>8</v>
       </c>
       <c r="D85" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>55</v>
+        <v>152</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="I85" s="1">
         <v>1</v>
@@ -3967,7 +3968,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B86" s="1">
         <v>1</v>
@@ -3976,25 +3977,56 @@
         <v>8</v>
       </c>
       <c r="D86" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="I86" s="1">
         <v>1</v>
       </c>
       <c r="J86" s="1"/>
       <c r="L86" s="1"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A87" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B87" s="1">
+        <v>1</v>
+      </c>
+      <c r="C87" s="1">
+        <v>8</v>
+      </c>
+      <c r="D87" s="1">
+        <v>4</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I87" s="1">
+        <v>1</v>
+      </c>
+      <c r="J87" s="1"/>
+      <c r="L87" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
Fix HW PTT visibility, add Init buttons, improve DISCO toggle and cached plans
- Always show HW PTT controls, default button index to 0, show index on Detect btn
- Add Init FMS/CL buttons to Control page for re-initialization without page switch
- Rename disco toggle from "skip" to "DISCO", invert logic (checked = remove discos)
- Deduplicate cached SimBrief plans using route+flight_number as cache key
- Add delete button (X) to cached plans dropdown with X-Plane .fms file sync
- Clean up old timestamp-based cache duplicates on save

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/CopilotAI_Checklists.xlsx
+++ b/CopilotAI_Checklists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnl\Documents\projects\CopilotAI\claude_shell_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069DAABC-7B0F-4B39-94AC-2734E9A61BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14A7894-B98D-4E1F-8F1D-B0E7D2EFF653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57840" yWindow="-98" windowWidth="28995" windowHeight="16395" xr2:uid="{B7C423D5-FDD5-4D99-96F7-653924CCE03F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="169">
   <si>
     <t>checklist</t>
   </si>
@@ -242,9 +242,6 @@
     <t>cmd:laminar/B738/rotary/eng1_start_off;</t>
   </si>
   <si>
-    <t>GPU  Disconnect</t>
-  </si>
-  <si>
     <t>Battery On</t>
   </si>
   <si>
@@ -269,18 +266,6 @@
     <t>Window Heat ON</t>
   </si>
   <si>
-    <t>Chock  Wheels</t>
-  </si>
-  <si>
-    <t>Open Exterior Doors and Hatches</t>
-  </si>
-  <si>
-    <t>Illuminate Cockpit</t>
-  </si>
-  <si>
-    <t>Connect Ground Power Unit</t>
-  </si>
-  <si>
     <t>wait</t>
   </si>
   <si>
@@ -305,9 +290,6 @@
     <t>WHITE DOME LIGHT</t>
   </si>
   <si>
-    <t>GPU On</t>
-  </si>
-  <si>
     <t>ICING WINDOW</t>
   </si>
   <si>
@@ -506,28 +488,58 @@
     <t>IRS_NAV</t>
   </si>
   <si>
-    <t>Command IRS switchs to align</t>
-  </si>
-  <si>
-    <t>cmd:laminar/B738/toggle_switch/irs_L_right; cmd:laminar/B738/toggle_switch/irs_R_right; cmd:sleep(2000);</t>
-  </si>
-  <si>
     <t>Initialize FMS Position and Flight Plan</t>
   </si>
   <si>
-    <t>Start APU and Wait till APU Power is Available</t>
-  </si>
-  <si>
     <t>cmd.sendCommand("laminar/B738/toggle_switch/apu_gen1_dn");</t>
   </si>
   <si>
     <t>cmd:laminar/B738/toggle_switch/apu_gen1_dn; cmd sleep (500); cmd:laminar/B738/toggle_switch/apu_gen2_dn;</t>
   </si>
   <si>
-    <t>Place both APU Generators online.</t>
-  </si>
-  <si>
     <t>cmd: laminar/B738/gpu_toggle</t>
+  </si>
+  <si>
+    <t>laminar/B738/irs/alignment_left_remain:&gt;-1</t>
+  </si>
+  <si>
+    <t>laminar/B738/irs/alignment_right_remain:&gt;-1</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/irs_L_right;</t>
+  </si>
+  <si>
+    <t>cmd:laminar/B738/toggle_switch/irs_R_right;</t>
+  </si>
+  <si>
+    <t>Opening Exterior Doors and Hatches</t>
+  </si>
+  <si>
+    <t>Chocking  Wheels</t>
+  </si>
+  <si>
+    <t>GPU Ready</t>
+  </si>
+  <si>
+    <t>GPU On Bus</t>
+  </si>
+  <si>
+    <t>Cockpit Dome light on</t>
+  </si>
+  <si>
+    <t>IRS Left switch on align</t>
+  </si>
+  <si>
+    <t>IRS Right switch on align</t>
+  </si>
+  <si>
+    <t>Starting APU - waiting for warmup</t>
+  </si>
+  <si>
+    <t>Both APU Generators online.</t>
+  </si>
+  <si>
+    <t>GPU  Disconnected</t>
   </si>
 </sst>
 </file>
@@ -1124,10 +1136,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}" name="ZIBO737" displayName="ZIBO737" ref="A1:L87" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L87" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L87">
-    <sortCondition ref="C1:C87"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}" name="ZIBO737" displayName="ZIBO737" ref="A1:L88" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L88" xr:uid="{A2870296-6B4B-44FD-92E3-3824DA5FD872}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L88">
+    <sortCondition ref="C1:C88"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{D7EB0E30-B8BB-40E3-B6DB-C78633A8AE10}" name="checklist" dataDxfId="11"/>
@@ -1464,11 +1476,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BB3736-AF94-49F8-BA64-38BE7B846CBA}">
-  <dimension ref="A1:N87"/>
+  <dimension ref="A1:N88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1517,7 +1529,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1526,7 +1538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -1545,7 +1557,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>79</v>
+        <v>159</v>
       </c>
       <c r="I2" s="1">
         <v>1</v>
@@ -1570,7 +1582,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1597,7 +1609,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1624,7 +1636,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1651,11 +1663,11 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
@@ -1707,11 +1719,11 @@
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>81</v>
+        <v>161</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>
@@ -1736,13 +1748,13 @@
         <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>90</v>
+        <v>162</v>
       </c>
       <c r="I9" s="1">
         <v>1</v>
@@ -1773,7 +1785,7 @@
         <v>14</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I10" s="1">
         <v>1</v>
@@ -1798,13 +1810,13 @@
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="I11" s="1">
         <v>1</v>
@@ -1829,13 +1841,13 @@
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I12" s="1">
         <v>1</v>
@@ -1843,7 +1855,7 @@
       <c r="J12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1862,17 +1874,20 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I13" s="1">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1"/>
-      <c r="L13" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1888,20 +1903,23 @@
       <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I14" s="1">
         <v>1</v>
       </c>
       <c r="J14" s="1"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K14" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1914,29 +1932,23 @@
       <c r="D15" s="1">
         <v>8</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="I15" s="1">
         <v>1</v>
       </c>
-      <c r="J15" s="1">
-        <v>1</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="N15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1949,13 +1961,11 @@
       <c r="D16" s="1">
         <v>9</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
       <c r="I16" s="1">
         <v>1</v>
@@ -1964,13 +1974,16 @@
         <v>1</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+      <c r="N16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1986,20 +1999,25 @@
       <c r="E17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>156</v>
-      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
       </c>
-      <c r="J17" s="1"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -2016,10 +2034,12 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="I18" s="1">
         <v>1</v>
       </c>
@@ -2042,20 +2062,15 @@
       <c r="E19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="H19" s="1"/>
       <c r="I19" s="1">
         <v>1</v>
       </c>
-      <c r="J19" s="1">
-        <v>1</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="J19" s="1"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
@@ -2074,17 +2089,20 @@
       <c r="E20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="I20" s="1">
         <v>1</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
@@ -2104,10 +2122,10 @@
         <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1">
@@ -2133,14 +2151,12 @@
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="H22" s="1"/>
       <c r="I22" s="1">
         <v>1</v>
       </c>
@@ -2163,20 +2179,19 @@
       <c r="E23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H23" s="1" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="I23" s="1">
         <v>1</v>
       </c>
-      <c r="J23" s="1">
-        <v>1</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="J23" s="1"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
@@ -2198,7 +2213,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I24" s="1">
         <v>1</v>
@@ -2207,13 +2222,11 @@
         <v>1</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
@@ -2232,7 +2245,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="I25" s="1">
         <v>1</v>
@@ -2241,9 +2254,11 @@
         <v>1</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L25" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
@@ -2264,7 +2279,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
@@ -2273,7 +2288,7 @@
         <v>1</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L26" s="1"/>
     </row>
@@ -2296,7 +2311,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="I27" s="1">
         <v>1</v>
@@ -2305,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L27" s="1"/>
     </row>
@@ -2325,13 +2340,11 @@
       <c r="E28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="I28" s="1">
         <v>1</v>
       </c>
@@ -2339,11 +2352,11 @@
         <v>1</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
@@ -2359,11 +2372,13 @@
       <c r="E29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="F29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="1"/>
       <c r="I29" s="1">
         <v>1</v>
       </c>
@@ -2371,7 +2386,7 @@
         <v>1</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L29" s="1"/>
     </row>
@@ -2394,7 +2409,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="I30" s="1">
         <v>1</v>
@@ -2403,7 +2418,7 @@
         <v>1</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L30" s="1"/>
     </row>
@@ -2426,7 +2441,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="I31" s="1">
         <v>1</v>
@@ -2435,7 +2450,7 @@
         <v>1</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L31" s="1"/>
     </row>
@@ -2455,22 +2470,23 @@
       <c r="E32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I32" s="1">
         <v>1</v>
       </c>
-      <c r="J32" s="1"/>
+      <c r="J32" s="1">
+        <v>1</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
@@ -2487,13 +2503,13 @@
         <v>12</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="I33" s="1">
         <v>1</v>
@@ -2501,7 +2517,7 @@
       <c r="J33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
@@ -2517,20 +2533,19 @@
       <c r="E34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="H34" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="I34" s="1">
         <v>1</v>
       </c>
-      <c r="J34" s="1">
-        <v>1</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="J34" s="1"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.45">
@@ -2552,7 +2567,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="I35" s="1">
         <v>1</v>
@@ -2561,11 +2576,11 @@
         <v>1</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
@@ -2581,13 +2596,11 @@
       <c r="E36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="I36" s="1">
         <v>1</v>
       </c>
@@ -2595,11 +2608,11 @@
         <v>1</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>11</v>
       </c>
@@ -2615,11 +2628,13 @@
       <c r="E37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="F37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H37" s="1"/>
       <c r="I37" s="1">
         <v>1</v>
       </c>
@@ -2627,7 +2642,7 @@
         <v>1</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L37" s="1"/>
     </row>
@@ -2647,19 +2662,20 @@
       <c r="E38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
       <c r="H38" s="1" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="I38" s="1">
         <v>1</v>
       </c>
-      <c r="J38" s="1"/>
+      <c r="J38" s="1">
+        <v>1</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="L38" s="1"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.45">
@@ -2678,23 +2694,20 @@
       <c r="E39" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
+      <c r="F39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H39" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I39" s="1">
         <v>1</v>
       </c>
-      <c r="J39" s="1">
-        <v>1</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="J39" s="1"/>
+      <c r="L39" s="1"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
@@ -2714,7 +2727,9 @@
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="H40" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="I40" s="1">
         <v>1</v>
       </c>
@@ -2722,10 +2737,10 @@
         <v>1</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.45">
@@ -2754,10 +2769,10 @@
         <v>1</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.45">
@@ -2786,10 +2801,10 @@
         <v>1</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.45">
@@ -2808,23 +2823,23 @@
       <c r="E43" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1">
         <v>1</v>
       </c>
-      <c r="J43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="N43" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="J43" s="1">
+        <v>1</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>11</v>
       </c>
@@ -2840,26 +2855,23 @@
       <c r="E44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="F44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="1"/>
       <c r="I44" s="1">
         <v>1</v>
       </c>
-      <c r="J44" s="1">
-        <v>1</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="J44" s="1"/>
       <c r="L44" s="1"/>
       <c r="N44" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>11</v>
       </c>
@@ -2875,20 +2887,23 @@
       <c r="E45" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I45" s="1">
         <v>1</v>
       </c>
-      <c r="J45" s="1"/>
+      <c r="J45" s="1">
+        <v>1</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="L45" s="1"/>
       <c r="N45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.45">
@@ -2905,36 +2920,53 @@
         <v>39</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
+      <c r="H46" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="I46" s="1">
         <v>1</v>
       </c>
       <c r="J46" s="1"/>
       <c r="L46" s="1"/>
       <c r="N46" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B47" s="1">
         <v>1</v>
       </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="C47" s="1">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1">
+        <v>40</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
+      <c r="I47" s="1">
+        <v>1</v>
+      </c>
       <c r="J47" s="1"/>
       <c r="L47" s="1"/>
+      <c r="N47" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A48" s="1"/>
@@ -2952,31 +2984,17 @@
       <c r="L48" s="1"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A49" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A49" s="1"/>
       <c r="B49" s="1">
         <v>1</v>
       </c>
-      <c r="C49" s="1">
-        <v>3</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I49" s="1">
-        <v>1</v>
-      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="L49" s="1"/>
     </row>
@@ -2991,16 +3009,18 @@
         <v>3</v>
       </c>
       <c r="D50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
+      <c r="H50" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="I50" s="1">
         <v>1</v>
       </c>
@@ -3008,17 +3028,29 @@
       <c r="L50" s="1"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="B51" s="1">
         <v>1</v>
       </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="C51" s="1">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
+      <c r="I51" s="1">
+        <v>1</v>
+      </c>
       <c r="J51" s="1"/>
       <c r="L51" s="1"/>
     </row>
@@ -3038,35 +3070,21 @@
       <c r="L52" s="1"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A53" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A53" s="1"/>
       <c r="B53" s="1">
         <v>1</v>
       </c>
-      <c r="C53" s="1">
-        <v>4</v>
-      </c>
-      <c r="D53" s="1">
-        <v>1</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
       <c r="H53" s="1"/>
-      <c r="I53" s="1">
-        <v>1</v>
-      </c>
+      <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="L53" s="1"/>
     </row>
-    <row r="54" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>37</v>
       </c>
@@ -3077,25 +3095,25 @@
         <v>4</v>
       </c>
       <c r="D54" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="F54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H54" s="1"/>
       <c r="I54" s="1">
         <v>1</v>
       </c>
       <c r="J54" s="1"/>
-      <c r="L54" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L54" s="1"/>
+    </row>
+    <row r="55" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
@@ -3106,7 +3124,7 @@
         <v>4</v>
       </c>
       <c r="D55" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>12</v>
@@ -3114,15 +3132,17 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I55" s="1">
         <v>1</v>
       </c>
       <c r="J55" s="1"/>
-      <c r="L55" s="1"/>
-    </row>
-    <row r="56" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="L55" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>37</v>
       </c>
@@ -3133,7 +3153,7 @@
         <v>4</v>
       </c>
       <c r="D56" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>12</v>
@@ -3141,20 +3161,13 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I56" s="1">
         <v>1</v>
       </c>
-      <c r="J56" s="1">
-        <v>1</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="J56" s="1"/>
+      <c r="L56" s="1"/>
     </row>
     <row r="57" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
@@ -3167,7 +3180,7 @@
         <v>4</v>
       </c>
       <c r="D57" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>12</v>
@@ -3175,7 +3188,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I57" s="1">
         <v>1</v>
@@ -3184,13 +3197,13 @@
         <v>1</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>37</v>
       </c>
@@ -3201,34 +3214,53 @@
         <v>4</v>
       </c>
       <c r="D58" s="1">
+        <v>5</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I58" s="1">
+        <v>1</v>
+      </c>
+      <c r="J58" s="1">
+        <v>1</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A59" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1">
+        <v>4</v>
+      </c>
+      <c r="D59" s="1">
         <v>6</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1">
-        <v>1</v>
-      </c>
-      <c r="J58" s="1"/>
-      <c r="L58" s="1"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
+      <c r="I59" s="1">
+        <v>1</v>
+      </c>
       <c r="J59" s="1"/>
       <c r="L59" s="1"/>
     </row>
@@ -3248,35 +3280,21 @@
       <c r="L60" s="1"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A61" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="A61" s="1"/>
       <c r="B61" s="1">
         <v>1</v>
       </c>
-      <c r="C61" s="1">
-        <v>5</v>
-      </c>
-      <c r="D61" s="1">
-        <v>1</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="1">
-        <v>1</v>
-      </c>
+      <c r="I61" s="1"/>
       <c r="J61" s="1"/>
       <c r="L61" s="1"/>
     </row>
-    <row r="62" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>40</v>
       </c>
@@ -3287,25 +3305,25 @@
         <v>5</v>
       </c>
       <c r="D62" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="F62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62" s="1"/>
       <c r="I62" s="1">
         <v>1</v>
       </c>
       <c r="J62" s="1"/>
-      <c r="L62" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L62" s="1"/>
+    </row>
+    <row r="63" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>40</v>
       </c>
@@ -3316,7 +3334,7 @@
         <v>5</v>
       </c>
       <c r="D63" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>12</v>
@@ -3324,15 +3342,17 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I63" s="1">
         <v>1</v>
       </c>
       <c r="J63" s="1"/>
-      <c r="L63" s="1"/>
-    </row>
-    <row r="64" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="L63" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>40</v>
       </c>
@@ -3343,7 +3363,7 @@
         <v>5</v>
       </c>
       <c r="D64" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>12</v>
@@ -3351,20 +3371,13 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I64" s="1">
         <v>1</v>
       </c>
-      <c r="J64" s="1">
-        <v>1</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="J64" s="1"/>
+      <c r="L64" s="1"/>
     </row>
     <row r="65" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
@@ -3377,7 +3390,7 @@
         <v>5</v>
       </c>
       <c r="D65" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>12</v>
@@ -3385,7 +3398,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I65" s="1">
         <v>1</v>
@@ -3394,13 +3407,13 @@
         <v>1</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>40</v>
       </c>
@@ -3411,34 +3424,53 @@
         <v>5</v>
       </c>
       <c r="D66" s="1">
+        <v>5</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I66" s="1">
+        <v>1</v>
+      </c>
+      <c r="J66" s="1">
+        <v>1</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" s="1">
+        <v>1</v>
+      </c>
+      <c r="C67" s="1">
+        <v>5</v>
+      </c>
+      <c r="D67" s="1">
         <v>6</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F67" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1">
-        <v>1</v>
-      </c>
-      <c r="J66" s="1"/>
-      <c r="L66" s="1"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1">
-        <v>1</v>
-      </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
+      <c r="I67" s="1">
+        <v>1</v>
+      </c>
       <c r="J67" s="1"/>
       <c r="L67" s="1"/>
     </row>
@@ -3458,33 +3490,17 @@
       <c r="L68" s="1"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A69" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="A69" s="1"/>
       <c r="B69" s="1">
         <v>1</v>
       </c>
-      <c r="C69" s="1">
-        <v>6</v>
-      </c>
-      <c r="D69" s="1">
-        <v>1</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I69" s="1">
-        <v>1</v>
-      </c>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
       <c r="J69" s="1"/>
       <c r="L69" s="1"/>
     </row>
@@ -3499,19 +3515,19 @@
         <v>6</v>
       </c>
       <c r="D70" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="I70" s="1">
         <v>1</v>
@@ -3530,18 +3546,20 @@
         <v>6</v>
       </c>
       <c r="D71" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H71" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="I71" s="1">
         <v>1</v>
       </c>
@@ -3559,26 +3577,23 @@
         <v>6</v>
       </c>
       <c r="D72" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="F72" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H72" s="1"/>
       <c r="I72" s="1">
         <v>1</v>
       </c>
       <c r="J72" s="1"/>
-      <c r="K72" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="L72" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="L72" s="1"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
@@ -3591,26 +3606,26 @@
         <v>6</v>
       </c>
       <c r="D73" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="I73" s="1">
         <v>1</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L73" s="1"/>
+        <v>149</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
@@ -3623,24 +3638,25 @@
         <v>6</v>
       </c>
       <c r="D74" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H74" s="1"/>
       <c r="I74" s="1">
         <v>1</v>
       </c>
       <c r="J74" s="1"/>
+      <c r="K74" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="L74" s="1"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.45">
@@ -3654,19 +3670,19 @@
         <v>6</v>
       </c>
       <c r="D75" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I75" s="1">
         <v>1</v>
@@ -3685,17 +3701,19 @@
         <v>6</v>
       </c>
       <c r="D76" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G76" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="H76" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="I76" s="1">
         <v>1</v>
@@ -3714,17 +3732,17 @@
         <v>6</v>
       </c>
       <c r="D77" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G77" s="1"/>
       <c r="H77" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="I77" s="1">
         <v>1</v>
@@ -3743,19 +3761,17 @@
         <v>6</v>
       </c>
       <c r="D78" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G78" s="1">
-        <v>5</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="G78" s="1"/>
       <c r="H78" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="I78" s="1">
         <v>1</v>
@@ -3774,19 +3790,19 @@
         <v>6</v>
       </c>
       <c r="D79" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
+      </c>
+      <c r="G79" s="1">
+        <v>5</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="I79" s="1">
         <v>1</v>
@@ -3805,19 +3821,19 @@
         <v>6</v>
       </c>
       <c r="D80" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="I80" s="1">
         <v>1</v>
@@ -3836,16 +3852,20 @@
         <v>6</v>
       </c>
       <c r="D81" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="I81" s="1">
         <v>1</v>
       </c>
@@ -3854,21 +3874,23 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B82" s="1">
+        <v>1</v>
+      </c>
+      <c r="C82" s="1">
+        <v>6</v>
+      </c>
+      <c r="D82" s="1">
+        <v>13</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B82" s="1">
-        <v>1</v>
-      </c>
-      <c r="C82" s="1">
-        <v>7</v>
-      </c>
-      <c r="D82" s="1">
-        <v>1</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1">
@@ -3888,14 +3910,12 @@
         <v>7</v>
       </c>
       <c r="D83" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1">
@@ -3906,29 +3926,25 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1</v>
+      </c>
+      <c r="C84" s="1">
+        <v>7</v>
+      </c>
+      <c r="D84" s="1">
+        <v>2</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B84" s="1">
-        <v>1</v>
-      </c>
-      <c r="C84" s="1">
-        <v>8</v>
-      </c>
-      <c r="D84" s="1">
-        <v>1</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>149</v>
-      </c>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
       <c r="I84" s="1">
         <v>1</v>
       </c>
@@ -3946,19 +3962,19 @@
         <v>8</v>
       </c>
       <c r="D85" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>152</v>
+        <v>50</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="I85" s="1">
         <v>1</v>
@@ -3977,19 +3993,19 @@
         <v>8</v>
       </c>
       <c r="D86" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>54</v>
+        <v>146</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="I86" s="1">
         <v>1</v>
@@ -4008,25 +4024,56 @@
         <v>8</v>
       </c>
       <c r="D87" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="I87" s="1">
         <v>1</v>
       </c>
       <c r="J87" s="1"/>
       <c r="L87" s="1"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A88" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B88" s="1">
+        <v>1</v>
+      </c>
+      <c r="C88" s="1">
+        <v>8</v>
+      </c>
+      <c r="D88" s="1">
+        <v>4</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I88" s="1">
+        <v>1</v>
+      </c>
+      <c r="J88" s="1"/>
+      <c r="L88" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>